<commit_message>
shared_energy_storage_data.py updated. Case study plot funtion added.
</commit_message>
<xml_diff>
--- a/data/HR1/A_BJ_35_1/A_BJ_35_1_2020.xlsx
+++ b/data/HR1/A_BJ_35_1/A_BJ_35_1_2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\shared-resources-planning-v3\data\HR1\A_BJ_35_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DD5F0F-C715-4066-B737-D4E9ADB102CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67225799-B0C2-4FA1-A3B0-0A2EB9F72144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1950" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="45" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="4" r:id="rId1"/>
@@ -627,8 +627,11 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Pc, 2020, Autumn"/>
@@ -656,7 +659,7 @@
       <sheetData sheetId="0">
         <row r="2">
           <cell r="B2">
-            <v>1.2500000000000001E-2</v>
+            <v>5.0000000000000001E-3</v>
           </cell>
         </row>
         <row r="4">
@@ -670,16 +673,16 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
       <sheetData sheetId="11">
         <row r="2">
           <cell r="B2">
@@ -5500,11 +5503,11 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -5799,7 +5802,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5824,10 +5827,10 @@
         <v>3</v>
       </c>
       <c r="B1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1">
         <v>0.2</v>
@@ -5850,7 +5853,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2">
         <v>0.95</v>
@@ -5870,7 +5873,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2">
         <v>1.1000000000000001</v>
@@ -13019,99 +13022,99 @@
       </c>
       <c r="B2" s="1">
         <f>'[1]Pc, 2020, Summer'!B2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.91847476928571425</v>
+        <v>1.0205275214285714</v>
       </c>
       <c r="C2" s="1">
         <f>'[1]Pc, 2020, Summer'!C2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.87024217178571428</v>
+        <v>0.96693574642857139</v>
       </c>
       <c r="D2" s="1">
         <f>'[1]Pc, 2020, Summer'!D2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.72634905321428578</v>
+        <v>0.80705450357142861</v>
       </c>
       <c r="E2" s="1">
         <f>'[1]Pc, 2020, Summer'!E2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.82296753428571423</v>
+        <v>0.91440837142857134</v>
       </c>
       <c r="F2" s="1">
         <f>'[1]Pc, 2020, Summer'!F2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.80707891821428579</v>
+        <v>0.89675435357142863</v>
       </c>
       <c r="G2" s="1">
         <f>'[1]Pc, 2020, Summer'!G2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.81055215642857148</v>
+        <v>0.90061350714285715</v>
       </c>
       <c r="H2" s="1">
         <f>'[1]Pc, 2020, Summer'!H2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.89427690642857161</v>
+        <v>0.9936410071428573</v>
       </c>
       <c r="I2" s="1">
         <f>'[1]Pc, 2020, Summer'!I2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.96651900321428574</v>
+        <v>1.0739100035714286</v>
       </c>
       <c r="J2" s="1">
         <f>'[1]Pc, 2020, Summer'!J2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.0076641425000001</v>
+        <v>1.1196268250000001</v>
       </c>
       <c r="K2" s="1">
         <f>'[1]Pc, 2020, Summer'!K2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.97919517214285723</v>
+        <v>1.0879946357142858</v>
       </c>
       <c r="L2" s="1">
         <f>'[1]Pc, 2020, Summer'!L2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.96644828892857138</v>
+        <v>1.073831432142857</v>
       </c>
       <c r="M2" s="1">
         <f>'[1]Pc, 2020, Summer'!M2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.0627672982142857</v>
+        <v>1.1808525535714285</v>
       </c>
       <c r="N2" s="1">
         <f>'[1]Pc, 2020, Summer'!N2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.0360481657142857</v>
+        <v>1.1511646285714285</v>
       </c>
       <c r="O2" s="1">
         <f>'[1]Pc, 2020, Summer'!O2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.0362222417857143</v>
+        <v>1.1513580464285715</v>
       </c>
       <c r="P2" s="1">
         <f>'[1]Pc, 2020, Summer'!P2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.0070924753571431</v>
+        <v>1.1189916392857144</v>
       </c>
       <c r="Q2" s="1">
         <f>'[1]Pc, 2020, Summer'!Q2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.99326372464285717</v>
+        <v>1.1036263607142858</v>
       </c>
       <c r="R2" s="1">
         <f>'[1]Pc, 2020, Summer'!R2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.99644386821428577</v>
+        <v>1.1071598535714287</v>
       </c>
       <c r="S2" s="1">
         <f>'[1]Pc, 2020, Summer'!S2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.89421749357142866</v>
+        <v>0.9935749928571429</v>
       </c>
       <c r="T2" s="1">
         <f>'[1]Pc, 2020, Summer'!T2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.0786267735714288</v>
+        <v>1.198474192857143</v>
       </c>
       <c r="U2" s="1">
         <f>'[1]Pc, 2020, Summer'!U2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.0941504910714286</v>
+        <v>1.2157227678571429</v>
       </c>
       <c r="V2" s="1">
         <f>'[1]Pc, 2020, Summer'!V2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.0238401510714288</v>
+        <v>1.137600167857143</v>
       </c>
       <c r="W2" s="1">
         <f>'[1]Pc, 2020, Summer'!W2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.046576352857143</v>
+        <v>1.1628626142857144</v>
       </c>
       <c r="X2" s="1">
         <f>'[1]Pc, 2020, Summer'!X2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.96904690714285713</v>
+        <v>1.0767187857142857</v>
       </c>
       <c r="Y2" s="1">
         <f>'[1]Pc, 2020, Summer'!Y2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.85462916785714294</v>
+        <v>0.94958796428571435</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -13120,99 +13123,99 @@
       </c>
       <c r="B3" s="1">
         <f>'[1]Pc, 2020, Summer'!B3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.77329235571428567</v>
+        <v>-0.85921372857142853</v>
       </c>
       <c r="C3" s="1">
         <f>'[1]Pc, 2020, Summer'!C3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-1.2590011510714285</v>
+        <v>-1.3988901678571428</v>
       </c>
       <c r="D3" s="1">
         <f>'[1]Pc, 2020, Summer'!D3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.66517269428571435</v>
+        <v>-0.73908077142857143</v>
       </c>
       <c r="E3" s="1">
         <f>'[1]Pc, 2020, Summer'!E3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.6354629228571429</v>
+        <v>-0.70606991428571431</v>
       </c>
       <c r="F3" s="1">
         <f>'[1]Pc, 2020, Summer'!F3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-1.0001513603571428</v>
+        <v>-1.1112792892857142</v>
       </c>
       <c r="G3" s="1">
         <f>'[1]Pc, 2020, Summer'!G3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-1.6653287153571428</v>
+        <v>-1.8503652392857142</v>
       </c>
       <c r="H3" s="1">
         <f>'[1]Pc, 2020, Summer'!H3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-1.348377984642857</v>
+        <v>-1.4981977607142856</v>
       </c>
       <c r="I3" s="1">
         <f>'[1]Pc, 2020, Summer'!I3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-1.0799295878571429</v>
+        <v>-1.1999217642857143</v>
       </c>
       <c r="J3" s="1">
         <f>'[1]Pc, 2020, Summer'!J3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.93129096857142868</v>
+        <v>-1.0347677428571429</v>
       </c>
       <c r="K3" s="1">
         <f>'[1]Pc, 2020, Summer'!K3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.90553443750000018</v>
+        <v>-1.0061493750000001</v>
       </c>
       <c r="L3" s="1">
         <f>'[1]Pc, 2020, Summer'!L3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.96817013357142867</v>
+        <v>-1.075744592857143</v>
       </c>
       <c r="M3" s="1">
         <f>'[1]Pc, 2020, Summer'!M3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.87876960750000011</v>
+        <v>-0.97641067500000012</v>
       </c>
       <c r="N3" s="1">
         <f>'[1]Pc, 2020, Summer'!N3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.91539851464285726</v>
+        <v>-1.0171094607142859</v>
       </c>
       <c r="O3" s="1">
         <f>'[1]Pc, 2020, Summer'!O3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-1.0086037200000002</v>
+        <v>-1.1206708000000001</v>
       </c>
       <c r="P3" s="1">
         <f>'[1]Pc, 2020, Summer'!P3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-1.1600669892857145</v>
+        <v>-1.2889633214285716</v>
       </c>
       <c r="Q3" s="1">
         <f>'[1]Pc, 2020, Summer'!Q3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-1.2830279946428571</v>
+        <v>-1.4255866607142857</v>
       </c>
       <c r="R3" s="1">
         <f>'[1]Pc, 2020, Summer'!R3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-1.34499123</v>
+        <v>-1.4944347</v>
       </c>
       <c r="S3" s="1">
         <f>'[1]Pc, 2020, Summer'!S3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-1.1893089085714288</v>
+        <v>-1.321454342857143</v>
       </c>
       <c r="T3" s="1">
         <f>'[1]Pc, 2020, Summer'!T3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-1.0486047792857143</v>
+        <v>-1.1651164214285714</v>
       </c>
       <c r="U3" s="1">
         <f>'[1]Pc, 2020, Summer'!U3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.4006769046428571</v>
+        <v>-0.44519656071428565</v>
       </c>
       <c r="V3" s="1">
         <f>'[1]Pc, 2020, Summer'!V3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.1797153139285714</v>
+        <v>-0.19968368214285712</v>
       </c>
       <c r="W3" s="1">
         <f>'[1]Pc, 2020, Summer'!W3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.55540491107142864</v>
+        <v>-0.61711656785714286</v>
       </c>
       <c r="X3" s="1">
         <f>'[1]Pc, 2020, Summer'!X3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-1.0110606107142857</v>
+        <v>-1.1234006785714286</v>
       </c>
       <c r="Y3" s="1">
         <f>'[1]Pc, 2020, Summer'!Y3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-1.3676646117857143</v>
+        <v>-1.5196273464285714</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -13221,99 +13224,99 @@
       </c>
       <c r="B4" s="1">
         <f>'[1]Pc, 2020, Summer'!B4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-6.1539235714285719E-2</v>
+        <v>-6.8376928571428575E-2</v>
       </c>
       <c r="C4" s="1">
         <f>'[1]Pc, 2020, Summer'!C4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.21439878750000002</v>
+        <v>-0.23822087500000003</v>
       </c>
       <c r="D4" s="1">
         <f>'[1]Pc, 2020, Summer'!D4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.7406698017857144</v>
+        <v>-0.82296644642857153</v>
       </c>
       <c r="E4" s="1">
         <f>'[1]Pc, 2020, Summer'!E4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>4.6753344642857145E-2</v>
+        <v>5.1948160714285714E-2</v>
       </c>
       <c r="F4" s="1">
         <f>'[1]Pc, 2020, Summer'!F4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.8071967142857141E-2</v>
+        <v>4.2302185714285713E-2</v>
       </c>
       <c r="G4" s="1">
         <f>'[1]Pc, 2020, Summer'!G4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.13949861464285712</v>
+        <v>0.15499846071428569</v>
       </c>
       <c r="H4" s="1">
         <f>'[1]Pc, 2020, Summer'!H4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.1425643103571429</v>
+        <v>-0.15840478928571433</v>
       </c>
       <c r="I4" s="1">
         <f>'[1]Pc, 2020, Summer'!I4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.49174421464285717</v>
+        <v>-0.54638246071428576</v>
       </c>
       <c r="J4" s="1">
         <f>'[1]Pc, 2020, Summer'!J4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.57458436428571424</v>
+        <v>-0.63842707142857136</v>
       </c>
       <c r="K4" s="1">
         <f>'[1]Pc, 2020, Summer'!K4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.38260667250000002</v>
+        <v>-0.42511852500000002</v>
       </c>
       <c r="L4" s="1">
         <f>'[1]Pc, 2020, Summer'!L4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.40379809500000008</v>
+        <v>-0.44866455000000005</v>
       </c>
       <c r="M4" s="1">
         <f>'[1]Pc, 2020, Summer'!M4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.45381474642857145</v>
+        <v>-0.50423860714285718</v>
       </c>
       <c r="N4" s="1">
         <f>'[1]Pc, 2020, Summer'!N4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.35223417321428568</v>
+        <v>-0.39137130357142852</v>
       </c>
       <c r="O4" s="1">
         <f>'[1]Pc, 2020, Summer'!O4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.4162085646428571</v>
+        <v>-0.46245396071428568</v>
       </c>
       <c r="P4" s="1">
         <f>'[1]Pc, 2020, Summer'!P4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.72116106107142863</v>
+        <v>-0.80129006785714296</v>
       </c>
       <c r="Q4" s="1">
         <f>'[1]Pc, 2020, Summer'!Q4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.20637702000000005</v>
+        <v>-0.22930780000000006</v>
       </c>
       <c r="R4" s="1">
         <f>'[1]Pc, 2020, Summer'!R4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.20571337928571429</v>
+        <v>-0.22857042142857142</v>
       </c>
       <c r="S4" s="1">
         <f>'[1]Pc, 2020, Summer'!S4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.22509890357142862</v>
+        <v>-0.25010989285714291</v>
       </c>
       <c r="T4" s="1">
         <f>'[1]Pc, 2020, Summer'!T4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.205127055</v>
+        <v>-0.22791895000000001</v>
       </c>
       <c r="U4" s="1">
         <f>'[1]Pc, 2020, Summer'!U4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.13220433000000001</v>
+        <v>-0.14689370000000002</v>
       </c>
       <c r="V4" s="1">
         <f>'[1]Pc, 2020, Summer'!V4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.21359042357142857</v>
+        <v>-0.23732269285714286</v>
       </c>
       <c r="W4" s="1">
         <f>'[1]Pc, 2020, Summer'!W4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.18506298214285716</v>
+        <v>-0.20562553571428571</v>
       </c>
       <c r="X4" s="1">
         <f>'[1]Pc, 2020, Summer'!X4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-3.6988293214285706E-2</v>
+        <v>-4.1098103571428561E-2</v>
       </c>
       <c r="Y4" s="1">
         <f>'[1]Pc, 2020, Summer'!Y4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>9.0993249642857182E-2</v>
+        <v>0.10110361071428575</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -13322,99 +13325,99 @@
       </c>
       <c r="B5" s="1">
         <f>'[1]Pc, 2020, Summer'!B5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.6524886467857143</v>
+        <v>1.8360984964285714</v>
       </c>
       <c r="C5" s="1">
         <f>'[1]Pc, 2020, Summer'!C5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.519923015</v>
+        <v>1.6888033499999999</v>
       </c>
       <c r="D5" s="1">
         <f>'[1]Pc, 2020, Summer'!D5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.4626361989285714</v>
+        <v>1.625151332142857</v>
       </c>
       <c r="E5" s="1">
         <f>'[1]Pc, 2020, Summer'!E5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.4590848471428572</v>
+        <v>1.6212053857142859</v>
       </c>
       <c r="F5" s="1">
         <f>'[1]Pc, 2020, Summer'!F5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.4404356096428574</v>
+        <v>1.6004840107142859</v>
       </c>
       <c r="G5" s="1">
         <f>'[1]Pc, 2020, Summer'!G5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.3663688978571431</v>
+        <v>1.5181876642857146</v>
       </c>
       <c r="H5" s="1">
         <f>'[1]Pc, 2020, Summer'!H5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.6544017446428572</v>
+        <v>1.8382241607142857</v>
       </c>
       <c r="I5" s="1">
         <f>'[1]Pc, 2020, Summer'!I5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.1396772800000003</v>
+        <v>2.3774192000000003</v>
       </c>
       <c r="J5" s="1">
         <f>'[1]Pc, 2020, Summer'!J5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.6279523321428573</v>
+        <v>2.9199470357142858</v>
       </c>
       <c r="K5" s="1">
         <f>'[1]Pc, 2020, Summer'!K5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.9524906285714283</v>
+        <v>3.2805451428571426</v>
       </c>
       <c r="L5" s="1">
         <f>'[1]Pc, 2020, Summer'!L5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.9122137578571428</v>
+        <v>3.2357930642857142</v>
       </c>
       <c r="M5" s="1">
         <f>'[1]Pc, 2020, Summer'!M5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.0778222339285715</v>
+        <v>3.419802482142857</v>
       </c>
       <c r="N5" s="1">
         <f>'[1]Pc, 2020, Summer'!N5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.0840887346428572</v>
+        <v>3.4267652607142858</v>
       </c>
       <c r="O5" s="1">
         <f>'[1]Pc, 2020, Summer'!O5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.9826865542857144</v>
+        <v>3.3140961714285715</v>
       </c>
       <c r="P5" s="1">
         <f>'[1]Pc, 2020, Summer'!P5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.8952707692857143</v>
+        <v>3.2169675214285713</v>
       </c>
       <c r="Q5" s="1">
         <f>'[1]Pc, 2020, Summer'!Q5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.6870552389285711</v>
+        <v>2.9856169321428569</v>
       </c>
       <c r="R5" s="1">
         <f>'[1]Pc, 2020, Summer'!R5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.6135156442857141</v>
+        <v>2.9039062714285713</v>
       </c>
       <c r="S5" s="1">
         <f>'[1]Pc, 2020, Summer'!S5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.6135156442857141</v>
+        <v>2.9039062714285713</v>
       </c>
       <c r="T5" s="1">
         <f>'[1]Pc, 2020, Summer'!T5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.6135156442857141</v>
+        <v>2.9039062714285713</v>
       </c>
       <c r="U5" s="1">
         <f>'[1]Pc, 2020, Summer'!U5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.6135156442857141</v>
+        <v>2.9039062714285713</v>
       </c>
       <c r="V5" s="1">
         <f>'[1]Pc, 2020, Summer'!V5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.6217522482142859</v>
+        <v>2.9130580535714286</v>
       </c>
       <c r="W5" s="1">
         <f>'[1]Pc, 2020, Summer'!W5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.6677567157142859</v>
+        <v>2.9641741285714285</v>
       </c>
       <c r="X5" s="1">
         <f>'[1]Pc, 2020, Summer'!X5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.4102213942857142</v>
+        <v>2.6780237714285713</v>
       </c>
       <c r="Y5" s="1">
         <f>'[1]Pc, 2020, Summer'!Y5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.0458359803571429</v>
+        <v>2.2731510892857143</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -13423,99 +13426,99 @@
       </c>
       <c r="B6" s="1">
         <f>'[1]Pc, 2020, Summer'!B6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.8156252021428569</v>
+        <v>2.0173613357142854</v>
       </c>
       <c r="C6" s="1">
         <f>'[1]Pc, 2020, Summer'!C6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.6101212817857142</v>
+        <v>1.7890236464285714</v>
       </c>
       <c r="D6" s="1">
         <f>'[1]Pc, 2020, Summer'!D6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.5044143982142857</v>
+        <v>1.6715715535714284</v>
       </c>
       <c r="E6" s="1">
         <f>'[1]Pc, 2020, Summer'!E6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.4587635600000002</v>
+        <v>1.6208484000000001</v>
       </c>
       <c r="F6" s="1">
         <f>'[1]Pc, 2020, Summer'!F6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.4824096746428572</v>
+        <v>1.6471218607142857</v>
       </c>
       <c r="G6" s="1">
         <f>'[1]Pc, 2020, Summer'!G6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.4840299800000001</v>
+        <v>1.6489222000000001</v>
       </c>
       <c r="H6" s="1">
         <f>'[1]Pc, 2020, Summer'!H6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.2376839435714286</v>
+        <v>2.4863154928571429</v>
       </c>
       <c r="I6" s="1">
         <f>'[1]Pc, 2020, Summer'!I6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.6571530732142858</v>
+        <v>2.9523923035714286</v>
       </c>
       <c r="J6" s="1">
         <f>'[1]Pc, 2020, Summer'!J6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.9826757349999999</v>
+        <v>3.3140841499999998</v>
       </c>
       <c r="K6" s="1">
         <f>'[1]Pc, 2020, Summer'!K6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.1090322089285709</v>
+        <v>3.4544802321428567</v>
       </c>
       <c r="L6" s="1">
         <f>'[1]Pc, 2020, Summer'!L6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.7376509021428572</v>
+        <v>3.0418343357142859</v>
       </c>
       <c r="M6" s="1">
         <f>'[1]Pc, 2020, Summer'!M6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.2544694285714288</v>
+        <v>3.6160771428571432</v>
       </c>
       <c r="N6" s="1">
         <f>'[1]Pc, 2020, Summer'!N6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.3005046889285716</v>
+        <v>3.6672274321428571</v>
       </c>
       <c r="O6" s="1">
         <f>'[1]Pc, 2020, Summer'!O6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.1214065017857142</v>
+        <v>3.4682294464285714</v>
       </c>
       <c r="P6" s="1">
         <f>'[1]Pc, 2020, Summer'!P6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.8260472853571432</v>
+        <v>3.1400525392857146</v>
       </c>
       <c r="Q6" s="1">
         <f>'[1]Pc, 2020, Summer'!Q6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.6955200796428564</v>
+        <v>2.995022310714285</v>
       </c>
       <c r="R6" s="1">
         <f>'[1]Pc, 2020, Summer'!R6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.6808467271428569</v>
+        <v>2.9787185857142853</v>
       </c>
       <c r="S6" s="1">
         <f>'[1]Pc, 2020, Summer'!S6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.6381083982142859</v>
+        <v>2.9312315535714286</v>
       </c>
       <c r="T6" s="1">
         <f>'[1]Pc, 2020, Summer'!T6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.470753584642857</v>
+        <v>2.7452817607142856</v>
       </c>
       <c r="U6" s="1">
         <f>'[1]Pc, 2020, Summer'!U6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.6478727875000003</v>
+        <v>2.9420808750000003</v>
       </c>
       <c r="V6" s="1">
         <f>'[1]Pc, 2020, Summer'!V6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.8613252732142862</v>
+        <v>3.179250303571429</v>
       </c>
       <c r="W6" s="1">
         <f>'[1]Pc, 2020, Summer'!W6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.7416341832142854</v>
+        <v>3.0462602035714283</v>
       </c>
       <c r="X6" s="1">
         <f>'[1]Pc, 2020, Summer'!X6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.2931964932142854</v>
+        <v>2.5479961035714283</v>
       </c>
       <c r="Y6" s="1">
         <f>'[1]Pc, 2020, Summer'!Y6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.8978702010714283</v>
+        <v>2.1087446678571427</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
@@ -13524,99 +13527,99 @@
       </c>
       <c r="B7" s="1">
         <f>'[1]Pc, 2020, Summer'!B7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.37080837964285712</v>
+        <v>0.4120093107142857</v>
       </c>
       <c r="C7" s="1">
         <f>'[1]Pc, 2020, Summer'!C7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.35821244250000006</v>
+        <v>0.39801382500000004</v>
       </c>
       <c r="D7" s="1">
         <f>'[1]Pc, 2020, Summer'!D7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.37669257642857146</v>
+        <v>0.41854730714285715</v>
       </c>
       <c r="E7" s="1">
         <f>'[1]Pc, 2020, Summer'!E7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.37062064928571425</v>
+        <v>0.41180072142857138</v>
       </c>
       <c r="F7" s="1">
         <f>'[1]Pc, 2020, Summer'!F7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.39072595499999996</v>
+        <v>0.43413994999999994</v>
       </c>
       <c r="G7" s="1">
         <f>'[1]Pc, 2020, Summer'!G7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.36547726821428572</v>
+        <v>0.40608585357142857</v>
       </c>
       <c r="H7" s="1">
         <f>'[1]Pc, 2020, Summer'!H7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.34895696785714292</v>
+        <v>0.38772996428571432</v>
       </c>
       <c r="I7" s="1">
         <f>'[1]Pc, 2020, Summer'!I7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.5042808514285716</v>
+        <v>0.56031205714285726</v>
       </c>
       <c r="J7" s="1">
         <f>'[1]Pc, 2020, Summer'!J7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.63372129428571422</v>
+        <v>0.70413477142857139</v>
       </c>
       <c r="K7" s="1">
         <f>'[1]Pc, 2020, Summer'!K7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.66491871107142864</v>
+        <v>0.73879856785714293</v>
       </c>
       <c r="L7" s="1">
         <f>'[1]Pc, 2020, Summer'!L7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.65177187428571437</v>
+        <v>0.72419097142857147</v>
       </c>
       <c r="M7" s="1">
         <f>'[1]Pc, 2020, Summer'!M7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.59598280928571423</v>
+        <v>0.66220312142857141</v>
       </c>
       <c r="N7" s="1">
         <f>'[1]Pc, 2020, Summer'!N7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.54546910071428567</v>
+        <v>0.6060767785714285</v>
       </c>
       <c r="O7" s="1">
         <f>'[1]Pc, 2020, Summer'!O7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.52532738357142861</v>
+        <v>0.58369709285714289</v>
       </c>
       <c r="P7" s="1">
         <f>'[1]Pc, 2020, Summer'!P7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.52633014107142861</v>
+        <v>0.58481126785714288</v>
       </c>
       <c r="Q7" s="1">
         <f>'[1]Pc, 2020, Summer'!Q7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.56328829714285722</v>
+        <v>0.62587588571428576</v>
       </c>
       <c r="R7" s="1">
         <f>'[1]Pc, 2020, Summer'!R7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.57512738571428579</v>
+        <v>0.63903042857142867</v>
       </c>
       <c r="S7" s="1">
         <f>'[1]Pc, 2020, Summer'!S7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.5642989135714287</v>
+        <v>0.62699879285714299</v>
       </c>
       <c r="T7" s="1">
         <f>'[1]Pc, 2020, Summer'!T7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.54614384357142853</v>
+        <v>0.60682649285714274</v>
       </c>
       <c r="U7" s="1">
         <f>'[1]Pc, 2020, Summer'!U7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.64036967785714283</v>
+        <v>0.71152186428571429</v>
       </c>
       <c r="V7" s="1">
         <f>'[1]Pc, 2020, Summer'!V7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.77267703535714283</v>
+        <v>0.85853003928571425</v>
       </c>
       <c r="W7" s="1">
         <f>'[1]Pc, 2020, Summer'!W7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.83725942499999995</v>
+        <v>0.93028824999999993</v>
       </c>
       <c r="X7" s="1">
         <f>'[1]Pc, 2020, Summer'!X7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.69887659821428572</v>
+        <v>0.7765295535714285</v>
       </c>
       <c r="Y7" s="1">
         <f>'[1]Pc, 2020, Summer'!Y7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.44849661107142863</v>
+        <v>0.49832956785714289</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -13625,99 +13628,99 @@
       </c>
       <c r="B8" s="1">
         <f>'[1]Pc, 2020, Summer'!B8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.42881884714285712</v>
+        <v>0.47646538571428571</v>
       </c>
       <c r="C8" s="1">
         <f>'[1]Pc, 2020, Summer'!C8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.3735613542857143</v>
+        <v>0.41506817142857144</v>
       </c>
       <c r="D8" s="1">
         <f>'[1]Pc, 2020, Summer'!D8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.3735613542857143</v>
+        <v>0.41506817142857144</v>
       </c>
       <c r="E8" s="1">
         <f>'[1]Pc, 2020, Summer'!E8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.3735613542857143</v>
+        <v>0.41506817142857144</v>
       </c>
       <c r="F8" s="1">
         <f>'[1]Pc, 2020, Summer'!F8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.3735613542857143</v>
+        <v>0.41506817142857144</v>
       </c>
       <c r="G8" s="1">
         <f>'[1]Pc, 2020, Summer'!G8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.3735613542857143</v>
+        <v>0.41506817142857144</v>
       </c>
       <c r="H8" s="1">
         <f>'[1]Pc, 2020, Summer'!H8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.44938592999999999</v>
+        <v>0.49931769999999998</v>
       </c>
       <c r="I8" s="1">
         <f>'[1]Pc, 2020, Summer'!I8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.65231298964285722</v>
+        <v>0.72479221071428579</v>
       </c>
       <c r="J8" s="1">
         <f>'[1]Pc, 2020, Summer'!J8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.74697057321428573</v>
+        <v>0.82996730357142856</v>
       </c>
       <c r="K8" s="1">
         <f>'[1]Pc, 2020, Summer'!K8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.7508428810714286</v>
+        <v>0.83426986785714285</v>
       </c>
       <c r="L8" s="1">
         <f>'[1]Pc, 2020, Summer'!L8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.70908012642857132</v>
+        <v>0.78786680714285695</v>
       </c>
       <c r="M8" s="1">
         <f>'[1]Pc, 2020, Summer'!M8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.71012603892857151</v>
+        <v>0.78902893214285719</v>
       </c>
       <c r="N8" s="1">
         <f>'[1]Pc, 2020, Summer'!N8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.71694416571428576</v>
+        <v>0.79660462857142855</v>
       </c>
       <c r="O8" s="1">
         <f>'[1]Pc, 2020, Summer'!O8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.71694416571428576</v>
+        <v>0.79660462857142855</v>
       </c>
       <c r="P8" s="1">
         <f>'[1]Pc, 2020, Summer'!P8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.66789899678571418</v>
+        <v>0.74210999642857134</v>
       </c>
       <c r="Q8" s="1">
         <f>'[1]Pc, 2020, Summer'!Q8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.56765845285714289</v>
+        <v>0.63073161428571434</v>
       </c>
       <c r="R8" s="1">
         <f>'[1]Pc, 2020, Summer'!R8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.56765845285714289</v>
+        <v>0.63073161428571434</v>
       </c>
       <c r="S8" s="1">
         <f>'[1]Pc, 2020, Summer'!S8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.56765845285714289</v>
+        <v>0.63073161428571434</v>
       </c>
       <c r="T8" s="1">
         <f>'[1]Pc, 2020, Summer'!T8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.57882776464285723</v>
+        <v>0.64314196071428575</v>
       </c>
       <c r="U8" s="1">
         <f>'[1]Pc, 2020, Summer'!U8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.69855663857142858</v>
+        <v>0.77617404285714287</v>
       </c>
       <c r="V8" s="1">
         <f>'[1]Pc, 2020, Summer'!V8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.75897819642857145</v>
+        <v>0.84330910714285712</v>
       </c>
       <c r="W8" s="1">
         <f>'[1]Pc, 2020, Summer'!W8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.76508845714285711</v>
+        <v>0.8500982857142857</v>
       </c>
       <c r="X8" s="1">
         <f>'[1]Pc, 2020, Summer'!X8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.65074526999999993</v>
+        <v>0.72305029999999992</v>
       </c>
       <c r="Y8" s="1">
         <f>'[1]Pc, 2020, Summer'!Y8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.54038495892857141</v>
+        <v>0.60042773214285716</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
@@ -13726,99 +13729,99 @@
       </c>
       <c r="B9" s="1">
         <f>'[1]Pc, 2020, Summer'!B9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.60022163250000005</v>
+        <v>0.66691292499999999</v>
       </c>
       <c r="C9" s="1">
         <f>'[1]Pc, 2020, Summer'!C9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.54269636142857147</v>
+        <v>0.60299595714285714</v>
       </c>
       <c r="D9" s="1">
         <f>'[1]Pc, 2020, Summer'!D9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.52774106142857147</v>
+        <v>0.58637895714285715</v>
       </c>
       <c r="E9" s="1">
         <f>'[1]Pc, 2020, Summer'!E9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.52645823357142851</v>
+        <v>0.58495359285714277</v>
       </c>
       <c r="F9" s="1">
         <f>'[1]Pc, 2020, Summer'!F9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.52378691785714293</v>
+        <v>0.58198546428571429</v>
       </c>
       <c r="G9" s="1">
         <f>'[1]Pc, 2020, Summer'!G9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.5295041003571429</v>
+        <v>0.58833788928571429</v>
       </c>
       <c r="H9" s="1">
         <f>'[1]Pc, 2020, Summer'!H9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.54238230964285716</v>
+        <v>0.60264701071428572</v>
       </c>
       <c r="I9" s="1">
         <f>'[1]Pc, 2020, Summer'!I9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.58540147071428572</v>
+        <v>0.65044607857142855</v>
       </c>
       <c r="J9" s="1">
         <f>'[1]Pc, 2020, Summer'!J9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.67404947785714298</v>
+        <v>0.74894386428571436</v>
       </c>
       <c r="K9" s="1">
         <f>'[1]Pc, 2020, Summer'!K9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.74380249607142856</v>
+        <v>0.82644721785714281</v>
       </c>
       <c r="L9" s="1">
         <f>'[1]Pc, 2020, Summer'!L9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.80168142857142854</v>
+        <v>0.8907571428571428</v>
       </c>
       <c r="M9" s="1">
         <f>'[1]Pc, 2020, Summer'!M9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.80791555500000001</v>
+        <v>0.89768395000000001</v>
       </c>
       <c r="N9" s="1">
         <f>'[1]Pc, 2020, Summer'!N9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.81296619428571437</v>
+        <v>0.90329577142857154</v>
       </c>
       <c r="O9" s="1">
         <f>'[1]Pc, 2020, Summer'!O9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.76117305535714286</v>
+        <v>0.84574783928571429</v>
       </c>
       <c r="P9" s="1">
         <f>'[1]Pc, 2020, Summer'!P9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.70080804964285714</v>
+        <v>0.7786756107142857</v>
       </c>
       <c r="Q9" s="1">
         <f>'[1]Pc, 2020, Summer'!Q9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.69371619750000002</v>
+        <v>0.77079577499999996</v>
       </c>
       <c r="R9" s="1">
         <f>'[1]Pc, 2020, Summer'!R9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.67503131357142865</v>
+        <v>0.75003479285714292</v>
       </c>
       <c r="S9" s="1">
         <f>'[1]Pc, 2020, Summer'!S9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.66076816500000002</v>
+        <v>0.73418684999999995</v>
       </c>
       <c r="T9" s="1">
         <f>'[1]Pc, 2020, Summer'!T9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.66689663142857147</v>
+        <v>0.74099625714285722</v>
       </c>
       <c r="U9" s="1">
         <f>'[1]Pc, 2020, Summer'!U9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.6821945517857142</v>
+        <v>0.75799394642857132</v>
       </c>
       <c r="V9" s="1">
         <f>'[1]Pc, 2020, Summer'!V9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.77736429964285725</v>
+        <v>0.86373811071428586</v>
       </c>
       <c r="W9" s="1">
         <f>'[1]Pc, 2020, Summer'!W9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.81584523964285716</v>
+        <v>0.90649471071428567</v>
       </c>
       <c r="X9" s="1">
         <f>'[1]Pc, 2020, Summer'!X9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.75990659785714287</v>
+        <v>0.8443406642857143</v>
       </c>
       <c r="Y9" s="1">
         <f>'[1]Pc, 2020, Summer'!Y9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.62430198107142865</v>
+        <v>0.69366886785714288</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
@@ -13827,99 +13830,99 @@
       </c>
       <c r="B10" s="1">
         <f>'[1]Pc, 2020, Summer'!B10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.48017731821428578</v>
+        <v>0.53353035357142864</v>
       </c>
       <c r="C10" s="1">
         <f>'[1]Pc, 2020, Summer'!C10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.43415708464285718</v>
+        <v>0.48239676071428572</v>
       </c>
       <c r="D10" s="1">
         <f>'[1]Pc, 2020, Summer'!D10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.42219284142857144</v>
+        <v>0.46910315714285716</v>
       </c>
       <c r="E10" s="1">
         <f>'[1]Pc, 2020, Summer'!E10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.42116656821428572</v>
+        <v>0.46796285357142858</v>
       </c>
       <c r="F10" s="1">
         <f>'[1]Pc, 2020, Summer'!F10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.41902949249999999</v>
+        <v>0.46558832499999997</v>
       </c>
       <c r="G10" s="1">
         <f>'[1]Pc, 2020, Summer'!G10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.42360327000000003</v>
+        <v>0.47067030000000004</v>
       </c>
       <c r="H10" s="1">
         <f>'[1]Pc, 2020, Summer'!H10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.43390585928571429</v>
+        <v>0.48211762142857145</v>
       </c>
       <c r="I10" s="1">
         <f>'[1]Pc, 2020, Summer'!I10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.46832119071428568</v>
+        <v>0.52035687857142854</v>
       </c>
       <c r="J10" s="1">
         <f>'[1]Pc, 2020, Summer'!J10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.53923956428571429</v>
+        <v>0.59915507142857138</v>
       </c>
       <c r="K10" s="1">
         <f>'[1]Pc, 2020, Summer'!K10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.595041975</v>
+        <v>0.66115774999999999</v>
       </c>
       <c r="L10" s="1">
         <f>'[1]Pc, 2020, Summer'!L10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.64134513642857138</v>
+        <v>0.71260570714285709</v>
       </c>
       <c r="M10" s="1">
         <f>'[1]Pc, 2020, Summer'!M10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.64633243178571409</v>
+        <v>0.71814714642857125</v>
       </c>
       <c r="N10" s="1">
         <f>'[1]Pc, 2020, Summer'!N10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.65037295928571426</v>
+        <v>0.72263662142857132</v>
       </c>
       <c r="O10" s="1">
         <f>'[1]Pc, 2020, Summer'!O10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.60893845071428565</v>
+        <v>0.67659827857142851</v>
       </c>
       <c r="P10" s="1">
         <f>'[1]Pc, 2020, Summer'!P10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.56064644035714295</v>
+        <v>0.62294048928571433</v>
       </c>
       <c r="Q10" s="1">
         <f>'[1]Pc, 2020, Summer'!Q10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.55497294642857142</v>
+        <v>0.61663660714285717</v>
       </c>
       <c r="R10" s="1">
         <f>'[1]Pc, 2020, Summer'!R10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.5400250617857143</v>
+        <v>0.60002784642857143</v>
       </c>
       <c r="S10" s="1">
         <f>'[1]Pc, 2020, Summer'!S10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.52861452750000004</v>
+        <v>0.58734947500000001</v>
       </c>
       <c r="T10" s="1">
         <f>'[1]Pc, 2020, Summer'!T10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.53351729357142852</v>
+        <v>0.59279699285714282</v>
       </c>
       <c r="U10" s="1">
         <f>'[1]Pc, 2020, Summer'!U10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.54575564464285709</v>
+        <v>0.60639516071428567</v>
       </c>
       <c r="V10" s="1">
         <f>'[1]Pc, 2020, Summer'!V10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.62189145964285708</v>
+        <v>0.69099051071428563</v>
       </c>
       <c r="W10" s="1">
         <f>'[1]Pc, 2020, Summer'!W10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.65267617178571435</v>
+        <v>0.72519574642857143</v>
       </c>
       <c r="X10" s="1">
         <f>'[1]Pc, 2020, Summer'!X10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.60792528214285724</v>
+        <v>0.67547253571428578</v>
       </c>
       <c r="Y10" s="1">
         <f>'[1]Pc, 2020, Summer'!Y10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.4994415771428572</v>
+        <v>0.55493508571428574</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
@@ -13928,99 +13931,99 @@
       </c>
       <c r="B11" s="1">
         <f>'[1]Pc, 2020, Summer'!B11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.48017731821428578</v>
+        <v>0.53353035357142864</v>
       </c>
       <c r="C11" s="1">
         <f>'[1]Pc, 2020, Summer'!C11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.43415708464285718</v>
+        <v>0.48239676071428572</v>
       </c>
       <c r="D11" s="1">
         <f>'[1]Pc, 2020, Summer'!D11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.42219284142857144</v>
+        <v>0.46910315714285716</v>
       </c>
       <c r="E11" s="1">
         <f>'[1]Pc, 2020, Summer'!E11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.42116656821428572</v>
+        <v>0.46796285357142858</v>
       </c>
       <c r="F11" s="1">
         <f>'[1]Pc, 2020, Summer'!F11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.41902949249999999</v>
+        <v>0.46558832499999997</v>
       </c>
       <c r="G11" s="1">
         <f>'[1]Pc, 2020, Summer'!G11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.42360327000000003</v>
+        <v>0.47067030000000004</v>
       </c>
       <c r="H11" s="1">
         <f>'[1]Pc, 2020, Summer'!H11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.43390585928571429</v>
+        <v>0.48211762142857145</v>
       </c>
       <c r="I11" s="1">
         <f>'[1]Pc, 2020, Summer'!I11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.46832119071428568</v>
+        <v>0.52035687857142854</v>
       </c>
       <c r="J11" s="1">
         <f>'[1]Pc, 2020, Summer'!J11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.53923956428571429</v>
+        <v>0.59915507142857138</v>
       </c>
       <c r="K11" s="1">
         <f>'[1]Pc, 2020, Summer'!K11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.595041975</v>
+        <v>0.66115774999999999</v>
       </c>
       <c r="L11" s="1">
         <f>'[1]Pc, 2020, Summer'!L11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.64134513642857138</v>
+        <v>0.71260570714285709</v>
       </c>
       <c r="M11" s="1">
         <f>'[1]Pc, 2020, Summer'!M11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.64633243178571409</v>
+        <v>0.71814714642857125</v>
       </c>
       <c r="N11" s="1">
         <f>'[1]Pc, 2020, Summer'!N11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.65037295928571426</v>
+        <v>0.72263662142857132</v>
       </c>
       <c r="O11" s="1">
         <f>'[1]Pc, 2020, Summer'!O11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.60893845071428565</v>
+        <v>0.67659827857142851</v>
       </c>
       <c r="P11" s="1">
         <f>'[1]Pc, 2020, Summer'!P11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.56064644035714295</v>
+        <v>0.62294048928571433</v>
       </c>
       <c r="Q11" s="1">
         <f>'[1]Pc, 2020, Summer'!Q11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.55497294642857142</v>
+        <v>0.61663660714285717</v>
       </c>
       <c r="R11" s="1">
         <f>'[1]Pc, 2020, Summer'!R11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.5400250617857143</v>
+        <v>0.60002784642857143</v>
       </c>
       <c r="S11" s="1">
         <f>'[1]Pc, 2020, Summer'!S11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.52861452750000004</v>
+        <v>0.58734947500000001</v>
       </c>
       <c r="T11" s="1">
         <f>'[1]Pc, 2020, Summer'!T11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.53351729357142852</v>
+        <v>0.59279699285714282</v>
       </c>
       <c r="U11" s="1">
         <f>'[1]Pc, 2020, Summer'!U11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.54575564464285709</v>
+        <v>0.60639516071428567</v>
       </c>
       <c r="V11" s="1">
         <f>'[1]Pc, 2020, Summer'!V11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.62189145964285708</v>
+        <v>0.69099051071428563</v>
       </c>
       <c r="W11" s="1">
         <f>'[1]Pc, 2020, Summer'!W11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.65267617178571435</v>
+        <v>0.72519574642857143</v>
       </c>
       <c r="X11" s="1">
         <f>'[1]Pc, 2020, Summer'!X11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.60792528214285724</v>
+        <v>0.67547253571428578</v>
       </c>
       <c r="Y11" s="1">
         <f>'[1]Pc, 2020, Summer'!Y11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.4994415771428572</v>
+        <v>0.55493508571428574</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -14029,99 +14032,99 @@
       </c>
       <c r="B12" s="1">
         <f>'[1]Pc, 2020, Summer'!B12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.120349217142858</v>
+        <v>3.4670546857142863</v>
       </c>
       <c r="C12" s="1">
         <f>'[1]Pc, 2020, Summer'!C12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.7587595664285711</v>
+        <v>3.0652884071428566</v>
       </c>
       <c r="D12" s="1">
         <f>'[1]Pc, 2020, Summer'!D12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.6152616378571434</v>
+        <v>2.9058462642857146</v>
       </c>
       <c r="E12" s="1">
         <f>'[1]Pc, 2020, Summer'!E12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.4840443539285717</v>
+        <v>2.7600492821428575</v>
       </c>
       <c r="F12" s="1">
         <f>'[1]Pc, 2020, Summer'!F12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.4755316878571429</v>
+        <v>2.7505907642857141</v>
       </c>
       <c r="G12" s="1">
         <f>'[1]Pc, 2020, Summer'!G12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.4686917778571429</v>
+        <v>2.7429908642857144</v>
       </c>
       <c r="H12" s="1">
         <f>'[1]Pc, 2020, Summer'!H12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.9896711199999997</v>
+        <v>3.3218567999999995</v>
       </c>
       <c r="I12" s="1">
         <f>'[1]Pc, 2020, Summer'!I12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.6460847700000003</v>
+        <v>4.0512053000000003</v>
       </c>
       <c r="J12" s="1">
         <f>'[1]Pc, 2020, Summer'!J12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>4.1345633185714288</v>
+        <v>4.5939592428571432</v>
       </c>
       <c r="K12" s="1">
         <f>'[1]Pc, 2020, Summer'!K12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>4.2361468778571432</v>
+        <v>4.706829864285714</v>
       </c>
       <c r="L12" s="1">
         <f>'[1]Pc, 2020, Summer'!L12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>4.301859378214286</v>
+        <v>4.7798437535714289</v>
       </c>
       <c r="M12" s="1">
         <f>'[1]Pc, 2020, Summer'!M12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>4.5824820621428577</v>
+        <v>5.0916467357142858</v>
       </c>
       <c r="N12" s="1">
         <f>'[1]Pc, 2020, Summer'!N12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>4.6085436225000009</v>
+        <v>5.1206040250000004</v>
       </c>
       <c r="O12" s="1">
         <f>'[1]Pc, 2020, Summer'!O12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>4.5298283914285715</v>
+        <v>5.0331426571428572</v>
       </c>
       <c r="P12" s="1">
         <f>'[1]Pc, 2020, Summer'!P12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>4.394642997857142</v>
+        <v>4.8829366642857135</v>
       </c>
       <c r="Q12" s="1">
         <f>'[1]Pc, 2020, Summer'!Q12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>4.1896845128571423</v>
+        <v>4.6552050142857135</v>
       </c>
       <c r="R12" s="1">
         <f>'[1]Pc, 2020, Summer'!R12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>4.1515340560714282</v>
+        <v>4.6128156178571427</v>
       </c>
       <c r="S12" s="1">
         <f>'[1]Pc, 2020, Summer'!S12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>4.1330792250000004</v>
+        <v>4.5923102500000006</v>
       </c>
       <c r="T12" s="1">
         <f>'[1]Pc, 2020, Summer'!T12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>4.240161986785715</v>
+        <v>4.7112910964285719</v>
       </c>
       <c r="U12" s="1">
         <f>'[1]Pc, 2020, Summer'!U12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>4.4329225210714291</v>
+        <v>4.9254694678571429</v>
       </c>
       <c r="V12" s="1">
         <f>'[1]Pc, 2020, Summer'!V12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>4.5998365757142849</v>
+        <v>5.110929528571428</v>
       </c>
       <c r="W12" s="1">
         <f>'[1]Pc, 2020, Summer'!W12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>4.6974952317857142</v>
+        <v>5.219439146428571</v>
       </c>
       <c r="X12" s="1">
         <f>'[1]Pc, 2020, Summer'!X12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>4.3340272682142862</v>
+        <v>4.8155858535714291</v>
       </c>
       <c r="Y12" s="1">
         <f>'[1]Pc, 2020, Summer'!Y12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.7510460742857146</v>
+        <v>4.1678289714285714</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -14130,99 +14133,99 @@
       </c>
       <c r="B13" s="1">
         <f>'[1]Pc, 2020, Summer'!B13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.8790491178571429</v>
+        <v>3.1989434642857142</v>
       </c>
       <c r="C13" s="1">
         <f>'[1]Pc, 2020, Summer'!C13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.5867624371428568</v>
+        <v>2.8741804857142852</v>
       </c>
       <c r="D13" s="1">
         <f>'[1]Pc, 2020, Summer'!D13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.4234128453571429</v>
+        <v>2.6926809392857143</v>
       </c>
       <c r="E13" s="1">
         <f>'[1]Pc, 2020, Summer'!E13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.4033427521428576</v>
+        <v>2.670380835714286</v>
       </c>
       <c r="F13" s="1">
         <f>'[1]Pc, 2020, Summer'!F13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.4417451124999996</v>
+        <v>2.7130501249999996</v>
       </c>
       <c r="G13" s="1">
         <f>'[1]Pc, 2020, Summer'!G13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.4676155257142862</v>
+        <v>2.741795028571429</v>
       </c>
       <c r="H13" s="1">
         <f>'[1]Pc, 2020, Summer'!H13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.8761699696428571</v>
+        <v>3.1957444107142856</v>
       </c>
       <c r="I13" s="1">
         <f>'[1]Pc, 2020, Summer'!I13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.4935847939285711</v>
+        <v>3.8817608821428569</v>
       </c>
       <c r="J13" s="1">
         <f>'[1]Pc, 2020, Summer'!J13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.9494889835714284</v>
+        <v>4.3883210928571428</v>
       </c>
       <c r="K13" s="1">
         <f>'[1]Pc, 2020, Summer'!K13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>4.2009855782142855</v>
+        <v>4.667761753571428</v>
       </c>
       <c r="L13" s="1">
         <f>'[1]Pc, 2020, Summer'!L13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>4.3502167189285723</v>
+        <v>4.833574132142858</v>
       </c>
       <c r="M13" s="1">
         <f>'[1]Pc, 2020, Summer'!M13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>4.7063701574999994</v>
+        <v>5.2293001749999988</v>
       </c>
       <c r="N13" s="1">
         <f>'[1]Pc, 2020, Summer'!N13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>4.7500098042857148</v>
+        <v>5.2777886714285716</v>
       </c>
       <c r="O13" s="1">
         <f>'[1]Pc, 2020, Summer'!O13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>4.7479174939285711</v>
+        <v>5.2754638821428568</v>
       </c>
       <c r="P13" s="1">
         <f>'[1]Pc, 2020, Summer'!P13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>4.4820326667857149</v>
+        <v>4.9800362964285716</v>
       </c>
       <c r="Q13" s="1">
         <f>'[1]Pc, 2020, Summer'!Q13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>4.2374392714285722</v>
+        <v>4.7082658571428579</v>
       </c>
       <c r="R13" s="1">
         <f>'[1]Pc, 2020, Summer'!R13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.9786109778571435</v>
+        <v>4.4206788642857147</v>
       </c>
       <c r="S13" s="1">
         <f>'[1]Pc, 2020, Summer'!S13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.9092077060714283</v>
+        <v>4.3435641178571425</v>
       </c>
       <c r="T13" s="1">
         <f>'[1]Pc, 2020, Summer'!T13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.7712621732142857</v>
+        <v>4.1902913035714286</v>
       </c>
       <c r="U13" s="1">
         <f>'[1]Pc, 2020, Summer'!U13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.7745865610714286</v>
+        <v>4.1939850678571426</v>
       </c>
       <c r="V13" s="1">
         <f>'[1]Pc, 2020, Summer'!V13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.8168768475000001</v>
+        <v>4.2409742750000001</v>
       </c>
       <c r="W13" s="1">
         <f>'[1]Pc, 2020, Summer'!W13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.9272774914285713</v>
+        <v>4.3636416571428569</v>
       </c>
       <c r="X13" s="1">
         <f>'[1]Pc, 2020, Summer'!X13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.7278198257142861</v>
+        <v>4.1420220285714286</v>
       </c>
       <c r="Y13" s="1">
         <f>'[1]Pc, 2020, Summer'!Y13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.2070279760714286</v>
+        <v>3.5633644178571426</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -14231,99 +14234,99 @@
       </c>
       <c r="B14" s="1">
         <f>'[1]Pc, 2020, Summer'!B14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.9792750914285722</v>
+        <v>3.310305657142858</v>
       </c>
       <c r="C14" s="1">
         <f>'[1]Pc, 2020, Summer'!C14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.4224062464285714</v>
+        <v>3.8026736071428568</v>
       </c>
       <c r="D14" s="1">
         <f>'[1]Pc, 2020, Summer'!D14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.2445850696428571</v>
+        <v>2.4939834107142858</v>
       </c>
       <c r="E14" s="1">
         <f>'[1]Pc, 2020, Summer'!E14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.0505376410714282</v>
+        <v>3.3894862678571425</v>
       </c>
       <c r="F14" s="1">
         <f>'[1]Pc, 2020, Summer'!F14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.7950568332142858</v>
+        <v>3.1056187035714284</v>
       </c>
       <c r="G14" s="1">
         <f>'[1]Pc, 2020, Summer'!G14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.7285473796428574</v>
+        <v>3.0317193107142861</v>
       </c>
       <c r="H14" s="1">
         <f>'[1]Pc, 2020, Summer'!H14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.3303975717857139</v>
+        <v>3.700441746428571</v>
       </c>
       <c r="I14" s="1">
         <f>'[1]Pc, 2020, Summer'!I14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.2444001128571429</v>
+        <v>3.6048890142857144</v>
       </c>
       <c r="J14" s="1">
         <f>'[1]Pc, 2020, Summer'!J14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.5575987821428572</v>
+        <v>3.9528875357142859</v>
       </c>
       <c r="K14" s="1">
         <f>'[1]Pc, 2020, Summer'!K14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.623371013571429</v>
+        <v>4.0259677928571431</v>
       </c>
       <c r="L14" s="1">
         <f>'[1]Pc, 2020, Summer'!L14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.2763024803571432</v>
+        <v>3.6403360892857144</v>
       </c>
       <c r="M14" s="1">
         <f>'[1]Pc, 2020, Summer'!M14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.3667658774999998</v>
+        <v>3.7408509749999999</v>
       </c>
       <c r="N14" s="1">
         <f>'[1]Pc, 2020, Summer'!N14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.5288805310714286</v>
+        <v>3.9209783678571428</v>
       </c>
       <c r="O14" s="1">
         <f>'[1]Pc, 2020, Summer'!O14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.4617038817857142</v>
+        <v>3.8463376464285712</v>
       </c>
       <c r="P14" s="1">
         <f>'[1]Pc, 2020, Summer'!P14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.5472800507142854</v>
+        <v>3.9414222785714284</v>
       </c>
       <c r="Q14" s="1">
         <f>'[1]Pc, 2020, Summer'!Q14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.6942556950000007</v>
+        <v>4.1047285500000008</v>
       </c>
       <c r="R14" s="1">
         <f>'[1]Pc, 2020, Summer'!R14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.6954789460714279</v>
+        <v>4.1060877178571422</v>
       </c>
       <c r="S14" s="1">
         <f>'[1]Pc, 2020, Summer'!S14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.6618721939285717</v>
+        <v>4.0687468821428574</v>
       </c>
       <c r="T14" s="1">
         <f>'[1]Pc, 2020, Summer'!T14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.4125292157142852</v>
+        <v>3.7916991285714281</v>
       </c>
       <c r="U14" s="1">
         <f>'[1]Pc, 2020, Summer'!U14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.6711078621428572</v>
+        <v>4.0790087357142859</v>
       </c>
       <c r="V14" s="1">
         <f>'[1]Pc, 2020, Summer'!V14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.7047039203571432</v>
+        <v>4.1163376892857144</v>
       </c>
       <c r="W14" s="1">
         <f>'[1]Pc, 2020, Summer'!W14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.4480170064285716</v>
+        <v>3.8311300071428573</v>
       </c>
       <c r="X14" s="1">
         <f>'[1]Pc, 2020, Summer'!X14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.074279393571429</v>
+        <v>3.4158659928571433</v>
       </c>
       <c r="Y14" s="1">
         <f>'[1]Pc, 2020, Summer'!Y14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>3.4123823582142858</v>
+        <v>3.7915359535714286</v>
       </c>
     </row>
   </sheetData>
@@ -20049,99 +20052,99 @@
       </c>
       <c r="B2" s="1">
         <f>'[1]Qc, 2020, Summer'!B2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.27554243464285721</v>
+        <v>0.30615826071428576</v>
       </c>
       <c r="C2" s="1">
         <f>'[1]Qc, 2020, Summer'!C2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.26107267178571425</v>
+        <v>0.2900807464285714</v>
       </c>
       <c r="D2" s="1">
         <f>'[1]Qc, 2020, Summer'!D2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.21790472464285715</v>
+        <v>0.24211636071428572</v>
       </c>
       <c r="E2" s="1">
         <f>'[1]Qc, 2020, Summer'!E2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.24689026607142853</v>
+        <v>0.27432251785714279</v>
       </c>
       <c r="F2" s="1">
         <f>'[1]Qc, 2020, Summer'!F2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.24212366357142859</v>
+        <v>0.26902629285714286</v>
       </c>
       <c r="G2" s="1">
         <f>'[1]Qc, 2020, Summer'!G2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.24316565142857138</v>
+        <v>0.27018405714285709</v>
       </c>
       <c r="H2" s="1">
         <f>'[1]Qc, 2020, Summer'!H2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.26828307642857147</v>
+        <v>0.29809230714285717</v>
       </c>
       <c r="I2" s="1">
         <f>'[1]Qc, 2020, Summer'!I2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.28995570964285711</v>
+        <v>0.32217301071428567</v>
       </c>
       <c r="J2" s="1">
         <f>'[1]Qc, 2020, Summer'!J2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.30229922892857142</v>
+        <v>0.33588803214285712</v>
       </c>
       <c r="K2" s="1">
         <f>'[1]Qc, 2020, Summer'!K2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.29375857285714291</v>
+        <v>0.32639841428571431</v>
       </c>
       <c r="L2" s="1">
         <f>'[1]Qc, 2020, Summer'!L2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.28993448249999998</v>
+        <v>0.32214942499999999</v>
       </c>
       <c r="M2" s="1">
         <f>'[1]Qc, 2020, Summer'!M2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.31883019107142857</v>
+        <v>0.35425576785714286</v>
       </c>
       <c r="N2" s="1">
         <f>'[1]Qc, 2020, Summer'!N2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.31081445357142856</v>
+        <v>0.34534939285714283</v>
       </c>
       <c r="O2" s="1">
         <f>'[1]Qc, 2020, Summer'!O2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.31086666642857147</v>
+        <v>0.34540740714285717</v>
       </c>
       <c r="P2" s="1">
         <f>'[1]Qc, 2020, Summer'!P2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.30212774357142852</v>
+        <v>0.33569749285714279</v>
       </c>
       <c r="Q2" s="1">
         <f>'[1]Qc, 2020, Summer'!Q2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.29797911964285717</v>
+        <v>0.33108791071428573</v>
       </c>
       <c r="R2" s="1">
         <f>'[1]Qc, 2020, Summer'!R2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.29893316785714286</v>
+        <v>0.3321479642857143</v>
       </c>
       <c r="S2" s="1">
         <f>'[1]Qc, 2020, Summer'!S2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.26826525000000001</v>
+        <v>0.29807250000000002</v>
       </c>
       <c r="T2" s="1">
         <f>'[1]Qc, 2020, Summer'!T2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.32358802178571427</v>
+        <v>0.35954224642857141</v>
       </c>
       <c r="U2" s="1">
         <f>'[1]Qc, 2020, Summer'!U2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.32824515535714294</v>
+        <v>0.36471683928571436</v>
       </c>
       <c r="V2" s="1">
         <f>'[1]Qc, 2020, Summer'!V2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.30715204821428577</v>
+        <v>0.3412800535714286</v>
       </c>
       <c r="W2" s="1">
         <f>'[1]Qc, 2020, Summer'!W2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.31397290071428569</v>
+        <v>0.34885877857142855</v>
       </c>
       <c r="X2" s="1">
         <f>'[1]Qc, 2020, Summer'!X2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.29071406571428571</v>
+        <v>0.32301562857142857</v>
       </c>
       <c r="Y2" s="1">
         <f>'[1]Qc, 2020, Summer'!Y2*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.25638875035714287</v>
+        <v>0.28487638928571429</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -20150,99 +20153,99 @@
       </c>
       <c r="B3" s="1">
         <f>'[1]Qc, 2020, Summer'!B3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.23198771250000003</v>
+        <v>-0.25776412500000001</v>
       </c>
       <c r="C3" s="1">
         <f>'[1]Qc, 2020, Summer'!C3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.37770032892857147</v>
+        <v>-0.41966703214285717</v>
       </c>
       <c r="D3" s="1">
         <f>'[1]Qc, 2020, Summer'!D3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.19955181214285714</v>
+        <v>-0.22172423571428571</v>
       </c>
       <c r="E3" s="1">
         <f>'[1]Qc, 2020, Summer'!E3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.19063888714285715</v>
+        <v>-0.2118209857142857</v>
       </c>
       <c r="F3" s="1">
         <f>'[1]Qc, 2020, Summer'!F3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.30004541035714288</v>
+        <v>-0.33338378928571433</v>
       </c>
       <c r="G3" s="1">
         <f>'[1]Qc, 2020, Summer'!G3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.49959862392857152</v>
+        <v>-0.55510958214285722</v>
       </c>
       <c r="H3" s="1">
         <f>'[1]Qc, 2020, Summer'!H3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.40451339249999996</v>
+        <v>-0.44945932499999997</v>
       </c>
       <c r="I3" s="1">
         <f>'[1]Qc, 2020, Summer'!I3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.32397889178571432</v>
+        <v>-0.35997654642857146</v>
       </c>
       <c r="J3" s="1">
         <f>'[1]Qc, 2020, Summer'!J3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.27938730857142857</v>
+        <v>-0.31043034285714283</v>
       </c>
       <c r="K3" s="1">
         <f>'[1]Qc, 2020, Summer'!K3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.27166034892857149</v>
+        <v>-0.30184483214285718</v>
       </c>
       <c r="L3" s="1">
         <f>'[1]Qc, 2020, Summer'!L3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.29045105035714286</v>
+        <v>-0.32272338928571426</v>
       </c>
       <c r="M3" s="1">
         <f>'[1]Qc, 2020, Summer'!M3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.26363089607142859</v>
+        <v>-0.29292321785714287</v>
       </c>
       <c r="N3" s="1">
         <f>'[1]Qc, 2020, Summer'!N3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.27461957142857146</v>
+        <v>-0.30513285714285715</v>
       </c>
       <c r="O3" s="1">
         <f>'[1]Qc, 2020, Summer'!O3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.30258112821428568</v>
+        <v>-0.33620125357142855</v>
       </c>
       <c r="P3" s="1">
         <f>'[1]Qc, 2020, Summer'!P3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.34802010964285718</v>
+        <v>-0.38668901071428574</v>
       </c>
       <c r="Q3" s="1">
         <f>'[1]Qc, 2020, Summer'!Q3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.3849083903571428</v>
+        <v>-0.42767598928571421</v>
       </c>
       <c r="R3" s="1">
         <f>'[1]Qc, 2020, Summer'!R3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.4034973375</v>
+        <v>-0.448330375</v>
       </c>
       <c r="S3" s="1">
         <f>'[1]Qc, 2020, Summer'!S3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.35679269250000001</v>
+        <v>-0.39643632499999998</v>
       </c>
       <c r="T3" s="1">
         <f>'[1]Qc, 2020, Summer'!T3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.31458143571428571</v>
+        <v>-0.34953492857142854</v>
       </c>
       <c r="U3" s="1">
         <f>'[1]Qc, 2020, Summer'!U3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.12020307107142858</v>
+        <v>-0.13355896785714286</v>
       </c>
       <c r="V3" s="1">
         <f>'[1]Qc, 2020, Summer'!V3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-5.39146125E-2</v>
+        <v>-5.9905124999999997E-2</v>
       </c>
       <c r="W3" s="1">
         <f>'[1]Qc, 2020, Summer'!W3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.16662147428571428</v>
+        <v>-0.18513497142857141</v>
       </c>
       <c r="X3" s="1">
         <f>'[1]Qc, 2020, Summer'!X3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.30331817035714281</v>
+        <v>-0.33702018928571426</v>
       </c>
       <c r="Y3" s="1">
         <f>'[1]Qc, 2020, Summer'!Y3*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.41029936714285709</v>
+        <v>-0.45588818571428563</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -20251,99 +20254,99 @@
       </c>
       <c r="B4" s="1">
         <f>'[1]Qc, 2020, Summer'!B4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-1.8461777142857148E-2</v>
+        <v>-2.0513085714285721E-2</v>
       </c>
       <c r="C4" s="1">
         <f>'[1]Qc, 2020, Summer'!C4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-6.431963142857143E-2</v>
+        <v>-7.1466257142857148E-2</v>
       </c>
       <c r="D4" s="1">
         <f>'[1]Qc, 2020, Summer'!D4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.22220093571428573</v>
+        <v>-0.24688992857142858</v>
       </c>
       <c r="E4" s="1">
         <f>'[1]Qc, 2020, Summer'!E4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.4025992142857144E-2</v>
+        <v>1.5584435714285715E-2</v>
       </c>
       <c r="F4" s="1">
         <f>'[1]Qc, 2020, Summer'!F4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.1421562499999999E-2</v>
+        <v>1.2690624999999999E-2</v>
       </c>
       <c r="G4" s="1">
         <f>'[1]Qc, 2020, Summer'!G4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>4.1849572500000001E-2</v>
+        <v>4.6499525E-2</v>
       </c>
       <c r="H4" s="1">
         <f>'[1]Qc, 2020, Summer'!H4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-4.2769282500000005E-2</v>
+        <v>-4.7521425000000006E-2</v>
       </c>
       <c r="I4" s="1">
         <f>'[1]Qc, 2020, Summer'!I4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.14752326535714286</v>
+        <v>-0.16391473928571429</v>
       </c>
       <c r="J4" s="1">
         <f>'[1]Qc, 2020, Summer'!J4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.17237531250000002</v>
+        <v>-0.19152812500000002</v>
       </c>
       <c r="K4" s="1">
         <f>'[1]Qc, 2020, Summer'!K4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.11478198535714283</v>
+        <v>-0.12753553928571426</v>
       </c>
       <c r="L4" s="1">
         <f>'[1]Qc, 2020, Summer'!L4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.12113942785714286</v>
+        <v>-0.13459936428571428</v>
       </c>
       <c r="M4" s="1">
         <f>'[1]Qc, 2020, Summer'!M4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.13614441750000003</v>
+        <v>-0.15127157500000002</v>
       </c>
       <c r="N4" s="1">
         <f>'[1]Qc, 2020, Summer'!N4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.10567025357142858</v>
+        <v>-0.11741139285714286</v>
       </c>
       <c r="O4" s="1">
         <f>'[1]Qc, 2020, Summer'!O4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.12486257357142858</v>
+        <v>-0.13873619285714286</v>
       </c>
       <c r="P4" s="1">
         <f>'[1]Qc, 2020, Summer'!P4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.21634832571428572</v>
+        <v>-0.24038702857142857</v>
       </c>
       <c r="Q4" s="1">
         <f>'[1]Qc, 2020, Summer'!Q4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-6.191310214285714E-2</v>
+        <v>-6.879233571428571E-2</v>
       </c>
       <c r="R4" s="1">
         <f>'[1]Qc, 2020, Summer'!R4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-6.1714028571428575E-2</v>
+        <v>-6.8571142857142858E-2</v>
       </c>
       <c r="S4" s="1">
         <f>'[1]Qc, 2020, Summer'!S4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-6.752967750000001E-2</v>
+        <v>-7.5032975000000002E-2</v>
       </c>
       <c r="T4" s="1">
         <f>'[1]Qc, 2020, Summer'!T4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-6.1538104285714289E-2</v>
+        <v>-6.8375671428571427E-2</v>
       </c>
       <c r="U4" s="1">
         <f>'[1]Qc, 2020, Summer'!U4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-3.9661315714285716E-2</v>
+        <v>-4.4068128571428569E-2</v>
       </c>
       <c r="V4" s="1">
         <f>'[1]Qc, 2020, Summer'!V4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-6.4077129642857139E-2</v>
+        <v>-7.1196810714285713E-2</v>
       </c>
       <c r="W4" s="1">
         <f>'[1]Qc, 2020, Summer'!W4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-5.5518891428571429E-2</v>
+        <v>-6.1687657142857143E-2</v>
       </c>
       <c r="X4" s="1">
         <f>'[1]Qc, 2020, Summer'!X4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-1.1096469642857142E-2</v>
+        <v>-1.2329410714285713E-2</v>
       </c>
       <c r="Y4" s="1">
         <f>'[1]Qc, 2020, Summer'!Y4*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>2.7297957857142868E-2</v>
+        <v>3.0331064285714297E-2</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -20352,99 +20355,99 @@
       </c>
       <c r="B5" s="1">
         <f>'[1]Qc, 2020, Summer'!B5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.32002232142857145</v>
+        <v>0.35558035714285718</v>
       </c>
       <c r="C5" s="1">
         <f>'[1]Qc, 2020, Summer'!C5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.2775237203571429</v>
+        <v>0.30835968928571433</v>
       </c>
       <c r="D5" s="1">
         <f>'[1]Qc, 2020, Summer'!D5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.10024682142857143</v>
+        <v>0.11138535714285713</v>
       </c>
       <c r="E5" s="1">
         <f>'[1]Qc, 2020, Summer'!E5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>7.7745535714285718E-2</v>
+        <v>8.638392857142857E-2</v>
       </c>
       <c r="F5" s="1">
         <f>'[1]Qc, 2020, Summer'!F5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>7.7745535714285718E-2</v>
+        <v>8.638392857142857E-2</v>
       </c>
       <c r="G5" s="1">
         <f>'[1]Qc, 2020, Summer'!G5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>7.7745535714285718E-2</v>
+        <v>8.638392857142857E-2</v>
       </c>
       <c r="H5" s="1">
         <f>'[1]Qc, 2020, Summer'!H5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.10446917142857144</v>
+        <v>0.11607685714285715</v>
       </c>
       <c r="I5" s="1">
         <f>'[1]Qc, 2020, Summer'!I5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.38008962321428574</v>
+        <v>0.42232180357142862</v>
       </c>
       <c r="J5" s="1">
         <f>'[1]Qc, 2020, Summer'!J5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.46013608928571431</v>
+        <v>0.51126232142857142</v>
       </c>
       <c r="K5" s="1">
         <f>'[1]Qc, 2020, Summer'!K5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.49178571428571433</v>
+        <v>0.54642857142857149</v>
       </c>
       <c r="L5" s="1">
         <f>'[1]Qc, 2020, Summer'!L5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.49178571428571433</v>
+        <v>0.54642857142857149</v>
       </c>
       <c r="M5" s="1">
         <f>'[1]Qc, 2020, Summer'!M5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.49178571428571433</v>
+        <v>0.54642857142857149</v>
       </c>
       <c r="N5" s="1">
         <f>'[1]Qc, 2020, Summer'!N5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.49178571428571433</v>
+        <v>0.54642857142857149</v>
       </c>
       <c r="O5" s="1">
         <f>'[1]Qc, 2020, Summer'!O5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.49178571428571433</v>
+        <v>0.54642857142857149</v>
       </c>
       <c r="P5" s="1">
         <f>'[1]Qc, 2020, Summer'!P5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.49178571428571433</v>
+        <v>0.54642857142857149</v>
       </c>
       <c r="Q5" s="1">
         <f>'[1]Qc, 2020, Summer'!Q5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.49178571428571433</v>
+        <v>0.54642857142857149</v>
       </c>
       <c r="R5" s="1">
         <f>'[1]Qc, 2020, Summer'!R5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.49178571428571433</v>
+        <v>0.54642857142857149</v>
       </c>
       <c r="S5" s="1">
         <f>'[1]Qc, 2020, Summer'!S5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.49178571428571433</v>
+        <v>0.54642857142857149</v>
       </c>
       <c r="T5" s="1">
         <f>'[1]Qc, 2020, Summer'!T5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.49178571428571433</v>
+        <v>0.54642857142857149</v>
       </c>
       <c r="U5" s="1">
         <f>'[1]Qc, 2020, Summer'!U5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.49178571428571433</v>
+        <v>0.54642857142857149</v>
       </c>
       <c r="V5" s="1">
         <f>'[1]Qc, 2020, Summer'!V5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.49178571428571433</v>
+        <v>0.54642857142857149</v>
       </c>
       <c r="W5" s="1">
         <f>'[1]Qc, 2020, Summer'!W5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.49178571428571433</v>
+        <v>0.54642857142857149</v>
       </c>
       <c r="X5" s="1">
         <f>'[1]Qc, 2020, Summer'!X5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.49178571428571433</v>
+        <v>0.54642857142857149</v>
       </c>
       <c r="Y5" s="1">
         <f>'[1]Qc, 2020, Summer'!Y5*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.44083008964285725</v>
+        <v>0.48981121071428579</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -20453,99 +20456,99 @@
       </c>
       <c r="B6" s="1">
         <f>'[1]Qc, 2020, Summer'!B6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.54468756964285714</v>
+        <v>0.60520841071428566</v>
       </c>
       <c r="C6" s="1">
         <f>'[1]Qc, 2020, Summer'!C6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.48303639000000009</v>
+        <v>0.5367071000000001</v>
       </c>
       <c r="D6" s="1">
         <f>'[1]Qc, 2020, Summer'!D6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.45132431464285716</v>
+        <v>0.50147146071428572</v>
       </c>
       <c r="E6" s="1">
         <f>'[1]Qc, 2020, Summer'!E6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.43762904678571429</v>
+        <v>0.48625449642857144</v>
       </c>
       <c r="F6" s="1">
         <f>'[1]Qc, 2020, Summer'!F6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.44472288535714283</v>
+        <v>0.49413653928571422</v>
       </c>
       <c r="G6" s="1">
         <f>'[1]Qc, 2020, Summer'!G6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.44520898821428573</v>
+        <v>0.49467665357142859</v>
       </c>
       <c r="H6" s="1">
         <f>'[1]Qc, 2020, Summer'!H6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.6713051817857143</v>
+        <v>0.7458946464285714</v>
       </c>
       <c r="I6" s="1">
         <f>'[1]Qc, 2020, Summer'!I6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.79714592357142855</v>
+        <v>0.88571769285714286</v>
       </c>
       <c r="J6" s="1">
         <f>'[1]Qc, 2020, Summer'!J6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.89480272178571429</v>
+        <v>0.99422524642857146</v>
       </c>
       <c r="K6" s="1">
         <f>'[1]Qc, 2020, Summer'!K6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.93270966107142872</v>
+        <v>1.0363440678571429</v>
       </c>
       <c r="L6" s="1">
         <f>'[1]Qc, 2020, Summer'!L6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.82129526678571441</v>
+        <v>0.91255029642857155</v>
       </c>
       <c r="M6" s="1">
         <f>'[1]Qc, 2020, Summer'!M6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.97634080928571443</v>
+        <v>1.0848231214285715</v>
       </c>
       <c r="N6" s="1">
         <f>'[1]Qc, 2020, Summer'!N6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.99015141214285718</v>
+        <v>1.1001682357142857</v>
       </c>
       <c r="O6" s="1">
         <f>'[1]Qc, 2020, Summer'!O6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.93642194892857133</v>
+        <v>1.040468832142857</v>
       </c>
       <c r="P6" s="1">
         <f>'[1]Qc, 2020, Summer'!P6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.84781418464285729</v>
+        <v>0.94201576071428583</v>
       </c>
       <c r="Q6" s="1">
         <f>'[1]Qc, 2020, Summer'!Q6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.80865602678571424</v>
+        <v>0.89850669642857139</v>
       </c>
       <c r="R6" s="1">
         <f>'[1]Qc, 2020, Summer'!R6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.80425401107142869</v>
+        <v>0.89361556785714291</v>
       </c>
       <c r="S6" s="1">
         <f>'[1]Qc, 2020, Summer'!S6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.79143251142857152</v>
+        <v>0.87936945714285719</v>
       </c>
       <c r="T6" s="1">
         <f>'[1]Qc, 2020, Summer'!T6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.74122607571428578</v>
+        <v>0.82358452857142861</v>
       </c>
       <c r="U6" s="1">
         <f>'[1]Qc, 2020, Summer'!U6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.79436182500000008</v>
+        <v>0.88262425000000011</v>
       </c>
       <c r="V6" s="1">
         <f>'[1]Qc, 2020, Summer'!V6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.85839757392857141</v>
+        <v>0.95377508214285711</v>
       </c>
       <c r="W6" s="1">
         <f>'[1]Qc, 2020, Summer'!W6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.82249026107142864</v>
+        <v>0.91387806785714287</v>
       </c>
       <c r="X6" s="1">
         <f>'[1]Qc, 2020, Summer'!X6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.68795895214285718</v>
+        <v>0.76439883571428568</v>
       </c>
       <c r="Y6" s="1">
         <f>'[1]Qc, 2020, Summer'!Y6*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.56936105678571436</v>
+        <v>0.63262339642857146</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
@@ -20554,99 +20557,99 @@
       </c>
       <c r="B7" s="1">
         <f>'[1]Qc, 2020, Summer'!B7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.22248504642857145</v>
+        <v>0.24720560714285716</v>
       </c>
       <c r="C7" s="1">
         <f>'[1]Qc, 2020, Summer'!C7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.21492747000000004</v>
+        <v>0.23880830000000003</v>
       </c>
       <c r="D7" s="1">
         <f>'[1]Qc, 2020, Summer'!D7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.226015515</v>
+        <v>0.25112835</v>
       </c>
       <c r="E7" s="1">
         <f>'[1]Qc, 2020, Summer'!E7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.22237237928571429</v>
+        <v>0.24708042142857142</v>
       </c>
       <c r="F7" s="1">
         <f>'[1]Qc, 2020, Summer'!F7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.23443557428571429</v>
+        <v>0.26048397142857144</v>
       </c>
       <c r="G7" s="1">
         <f>'[1]Qc, 2020, Summer'!G7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.21928637571428572</v>
+        <v>0.24365152857142858</v>
       </c>
       <c r="H7" s="1">
         <f>'[1]Qc, 2020, Summer'!H7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.20937420321428574</v>
+        <v>0.23263800357142858</v>
       </c>
       <c r="I7" s="1">
         <f>'[1]Qc, 2020, Summer'!I7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.30256853464285716</v>
+        <v>0.33618726071428573</v>
       </c>
       <c r="J7" s="1">
         <f>'[1]Qc, 2020, Summer'!J7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.38023277785714288</v>
+        <v>0.4224808642857143</v>
       </c>
       <c r="K7" s="1">
         <f>'[1]Qc, 2020, Summer'!K7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.39895123178571434</v>
+        <v>0.44327914642857147</v>
       </c>
       <c r="L7" s="1">
         <f>'[1]Qc, 2020, Summer'!L7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.3910631367857143</v>
+        <v>0.43451459642857143</v>
       </c>
       <c r="M7" s="1">
         <f>'[1]Qc, 2020, Summer'!M7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.35758969714285715</v>
+        <v>0.39732188571428573</v>
       </c>
       <c r="N7" s="1">
         <f>'[1]Qc, 2020, Summer'!N7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.3272814578571428</v>
+        <v>0.36364606428571422</v>
       </c>
       <c r="O7" s="1">
         <f>'[1]Qc, 2020, Summer'!O7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.31519642821428573</v>
+        <v>0.35021825357142861</v>
       </c>
       <c r="P7" s="1">
         <f>'[1]Qc, 2020, Summer'!P7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.31579808464285708</v>
+        <v>0.35088676071428565</v>
       </c>
       <c r="Q7" s="1">
         <f>'[1]Qc, 2020, Summer'!Q7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.33797297250000002</v>
+        <v>0.37552552500000003</v>
       </c>
       <c r="R7" s="1">
         <f>'[1]Qc, 2020, Summer'!R7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.34507644107142854</v>
+        <v>0.38341826785714284</v>
       </c>
       <c r="S7" s="1">
         <f>'[1]Qc, 2020, Summer'!S7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.33857933785714289</v>
+        <v>0.37619926428571432</v>
       </c>
       <c r="T7" s="1">
         <f>'[1]Qc, 2020, Summer'!T7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.32768632285714283</v>
+        <v>0.36409591428571425</v>
       </c>
       <c r="U7" s="1">
         <f>'[1]Qc, 2020, Summer'!U7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.38422181250000004</v>
+        <v>0.426913125</v>
       </c>
       <c r="V7" s="1">
         <f>'[1]Qc, 2020, Summer'!V7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.46360621285714293</v>
+        <v>0.51511801428571435</v>
       </c>
       <c r="W7" s="1">
         <f>'[1]Qc, 2020, Summer'!W7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.50235564214285722</v>
+        <v>0.55817293571428572</v>
       </c>
       <c r="X7" s="1">
         <f>'[1]Qc, 2020, Summer'!X7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.41932596857142851</v>
+        <v>0.46591774285714277</v>
       </c>
       <c r="Y7" s="1">
         <f>'[1]Qc, 2020, Summer'!Y7*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.26909797178571426</v>
+        <v>0.29899774642857141</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -20655,99 +20658,99 @@
       </c>
       <c r="B8" s="1">
         <f>'[1]Qc, 2020, Summer'!B8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.12864564000000001</v>
+        <v>0.1429396</v>
       </c>
       <c r="C8" s="1">
         <f>'[1]Qc, 2020, Summer'!C8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.11206837285714286</v>
+        <v>0.12452041428571428</v>
       </c>
       <c r="D8" s="1">
         <f>'[1]Qc, 2020, Summer'!D8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.11206837285714286</v>
+        <v>0.12452041428571428</v>
       </c>
       <c r="E8" s="1">
         <f>'[1]Qc, 2020, Summer'!E8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.11206837285714286</v>
+        <v>0.12452041428571428</v>
       </c>
       <c r="F8" s="1">
         <f>'[1]Qc, 2020, Summer'!F8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.11206837285714286</v>
+        <v>0.12452041428571428</v>
       </c>
       <c r="G8" s="1">
         <f>'[1]Qc, 2020, Summer'!G8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.11206837285714286</v>
+        <v>0.12452041428571428</v>
       </c>
       <c r="H8" s="1">
         <f>'[1]Qc, 2020, Summer'!H8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.13481575392857142</v>
+        <v>0.14979528214285714</v>
       </c>
       <c r="I8" s="1">
         <f>'[1]Qc, 2020, Summer'!I8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.19569390428571429</v>
+        <v>0.21743767142857143</v>
       </c>
       <c r="J8" s="1">
         <f>'[1]Qc, 2020, Summer'!J8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.22409119607142855</v>
+        <v>0.24899021785714284</v>
       </c>
       <c r="K8" s="1">
         <f>'[1]Qc, 2020, Summer'!K8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.2252528807142857</v>
+        <v>0.25028097857142856</v>
       </c>
       <c r="L8" s="1">
         <f>'[1]Qc, 2020, Summer'!L8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.21272403535714285</v>
+        <v>0.23636003928571428</v>
       </c>
       <c r="M8" s="1">
         <f>'[1]Qc, 2020, Summer'!M8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.21303783000000001</v>
+        <v>0.23670869999999999</v>
       </c>
       <c r="N8" s="1">
         <f>'[1]Qc, 2020, Summer'!N8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.21508327285714288</v>
+        <v>0.23898141428571429</v>
       </c>
       <c r="O8" s="1">
         <f>'[1]Qc, 2020, Summer'!O8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.21508327285714288</v>
+        <v>0.23898141428571429</v>
       </c>
       <c r="P8" s="1">
         <f>'[1]Qc, 2020, Summer'!P8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.20036972571428574</v>
+        <v>0.22263302857142858</v>
       </c>
       <c r="Q8" s="1">
         <f>'[1]Qc, 2020, Summer'!Q8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.17029756285714284</v>
+        <v>0.18921951428571426</v>
       </c>
       <c r="R8" s="1">
         <f>'[1]Qc, 2020, Summer'!R8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.17029756285714284</v>
+        <v>0.18921951428571426</v>
       </c>
       <c r="S8" s="1">
         <f>'[1]Qc, 2020, Summer'!S8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.17029756285714284</v>
+        <v>0.18921951428571426</v>
       </c>
       <c r="T8" s="1">
         <f>'[1]Qc, 2020, Summer'!T8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.17364835285714283</v>
+        <v>0.19294261428571427</v>
       </c>
       <c r="U8" s="1">
         <f>'[1]Qc, 2020, Summer'!U8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.20956697357142859</v>
+        <v>0.23285219285714287</v>
       </c>
       <c r="V8" s="1">
         <f>'[1]Qc, 2020, Summer'!V8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.2276934235714286</v>
+        <v>0.25299269285714288</v>
       </c>
       <c r="W8" s="1">
         <f>'[1]Qc, 2020, Summer'!W8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.22952650178571432</v>
+        <v>0.25502944642857145</v>
       </c>
       <c r="X8" s="1">
         <f>'[1]Qc, 2020, Summer'!X8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.19522357714285715</v>
+        <v>0.21691508571428572</v>
       </c>
       <c r="Y8" s="1">
         <f>'[1]Qc, 2020, Summer'!Y8*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.16211550535714286</v>
+        <v>0.18012833928571428</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
@@ -20756,99 +20759,99 @@
       </c>
       <c r="B9" s="1">
         <f>'[1]Qc, 2020, Summer'!B9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.60022163250000005</v>
+        <v>0.66691292499999999</v>
       </c>
       <c r="C9" s="1">
         <f>'[1]Qc, 2020, Summer'!C9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.54269636142857147</v>
+        <v>0.60299595714285714</v>
       </c>
       <c r="D9" s="1">
         <f>'[1]Qc, 2020, Summer'!D9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.52774106142857147</v>
+        <v>0.58637895714285715</v>
       </c>
       <c r="E9" s="1">
         <f>'[1]Qc, 2020, Summer'!E9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.52645823357142851</v>
+        <v>0.58495359285714277</v>
       </c>
       <c r="F9" s="1">
         <f>'[1]Qc, 2020, Summer'!F9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.52378691785714293</v>
+        <v>0.58198546428571429</v>
       </c>
       <c r="G9" s="1">
         <f>'[1]Qc, 2020, Summer'!G9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.5295041003571429</v>
+        <v>0.58833788928571429</v>
       </c>
       <c r="H9" s="1">
         <f>'[1]Qc, 2020, Summer'!H9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.54238230964285716</v>
+        <v>0.60264701071428572</v>
       </c>
       <c r="I9" s="1">
         <f>'[1]Qc, 2020, Summer'!I9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.58540147071428572</v>
+        <v>0.65044607857142855</v>
       </c>
       <c r="J9" s="1">
         <f>'[1]Qc, 2020, Summer'!J9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.67404947785714298</v>
+        <v>0.74894386428571436</v>
       </c>
       <c r="K9" s="1">
         <f>'[1]Qc, 2020, Summer'!K9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.74380249607142856</v>
+        <v>0.82644721785714281</v>
       </c>
       <c r="L9" s="1">
         <f>'[1]Qc, 2020, Summer'!L9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.80168142857142854</v>
+        <v>0.8907571428571428</v>
       </c>
       <c r="M9" s="1">
         <f>'[1]Qc, 2020, Summer'!M9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.80791555500000001</v>
+        <v>0.89768395000000001</v>
       </c>
       <c r="N9" s="1">
         <f>'[1]Qc, 2020, Summer'!N9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.81296619428571437</v>
+        <v>0.90329577142857154</v>
       </c>
       <c r="O9" s="1">
         <f>'[1]Qc, 2020, Summer'!O9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.76117305535714286</v>
+        <v>0.84574783928571429</v>
       </c>
       <c r="P9" s="1">
         <f>'[1]Qc, 2020, Summer'!P9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.70080804964285714</v>
+        <v>0.7786756107142857</v>
       </c>
       <c r="Q9" s="1">
         <f>'[1]Qc, 2020, Summer'!Q9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.69371619750000002</v>
+        <v>0.77079577499999996</v>
       </c>
       <c r="R9" s="1">
         <f>'[1]Qc, 2020, Summer'!R9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.67503131357142865</v>
+        <v>0.75003479285714292</v>
       </c>
       <c r="S9" s="1">
         <f>'[1]Qc, 2020, Summer'!S9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.66076816500000002</v>
+        <v>0.73418684999999995</v>
       </c>
       <c r="T9" s="1">
         <f>'[1]Qc, 2020, Summer'!T9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.66689663142857147</v>
+        <v>0.74099625714285722</v>
       </c>
       <c r="U9" s="1">
         <f>'[1]Qc, 2020, Summer'!U9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.6821945517857142</v>
+        <v>0.75799394642857132</v>
       </c>
       <c r="V9" s="1">
         <f>'[1]Qc, 2020, Summer'!V9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.77736429964285725</v>
+        <v>0.86373811071428586</v>
       </c>
       <c r="W9" s="1">
         <f>'[1]Qc, 2020, Summer'!W9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.81584523964285716</v>
+        <v>0.90649471071428567</v>
       </c>
       <c r="X9" s="1">
         <f>'[1]Qc, 2020, Summer'!X9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.75990659785714287</v>
+        <v>0.8443406642857143</v>
       </c>
       <c r="Y9" s="1">
         <f>'[1]Qc, 2020, Summer'!Y9*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.62430198107142865</v>
+        <v>0.69366886785714288</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
@@ -20857,99 +20860,99 @@
       </c>
       <c r="B10" s="1">
         <f>'[1]Qc, 2020, Summer'!B10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.15501303642857142</v>
+        <v>-0.17223670714285713</v>
       </c>
       <c r="C10" s="1">
         <f>'[1]Qc, 2020, Summer'!C10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.14987603892857143</v>
+        <v>-0.16652893214285713</v>
       </c>
       <c r="D10" s="1">
         <f>'[1]Qc, 2020, Summer'!D10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.14686813928571427</v>
+        <v>-0.16318682142857141</v>
       </c>
       <c r="E10" s="1">
         <f>'[1]Qc, 2020, Summer'!E10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.14944318071428569</v>
+        <v>-0.16604797857142856</v>
       </c>
       <c r="F10" s="1">
         <f>'[1]Qc, 2020, Summer'!F10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.14088848464285714</v>
+        <v>-0.15654276071428572</v>
       </c>
       <c r="G10" s="1">
         <f>'[1]Qc, 2020, Summer'!G10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.13903134428571429</v>
+        <v>-0.15447927142857143</v>
       </c>
       <c r="H10" s="1">
         <f>'[1]Qc, 2020, Summer'!H10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.17750352857142856</v>
+        <v>-0.19722614285714285</v>
       </c>
       <c r="I10" s="1">
         <f>'[1]Qc, 2020, Summer'!I10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.15365615785714284</v>
+        <v>-0.17072906428571427</v>
       </c>
       <c r="J10" s="1">
         <f>'[1]Qc, 2020, Summer'!J10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.12690604928571428</v>
+        <v>-0.14100672142857143</v>
       </c>
       <c r="K10" s="1">
         <f>'[1]Qc, 2020, Summer'!K10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-8.9655287142857143E-2</v>
+        <v>-9.9616985714285705E-2</v>
       </c>
       <c r="L10" s="1">
         <f>'[1]Qc, 2020, Summer'!L10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.10276145035714288</v>
+        <v>-0.11417938928571431</v>
       </c>
       <c r="M10" s="1">
         <f>'[1]Qc, 2020, Summer'!M10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.10144734428571427</v>
+        <v>-0.11271927142857141</v>
       </c>
       <c r="N10" s="1">
         <f>'[1]Qc, 2020, Summer'!N10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.10097902285714284</v>
+        <v>-0.11219891428571427</v>
       </c>
       <c r="O10" s="1">
         <f>'[1]Qc, 2020, Summer'!O10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-9.678707035714286E-2</v>
+        <v>-0.10754118928571428</v>
       </c>
       <c r="P10" s="1">
         <f>'[1]Qc, 2020, Summer'!P10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.13302481821428572</v>
+        <v>-0.14780535357142857</v>
       </c>
       <c r="Q10" s="1">
         <f>'[1]Qc, 2020, Summer'!Q10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.12884849357142858</v>
+        <v>-0.14316499285714285</v>
       </c>
       <c r="R10" s="1">
         <f>'[1]Qc, 2020, Summer'!R10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.13198059000000001</v>
+        <v>-0.1466451</v>
       </c>
       <c r="S10" s="1">
         <f>'[1]Qc, 2020, Summer'!S10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.13797887785714288</v>
+        <v>-0.1533098642857143</v>
       </c>
       <c r="T10" s="1">
         <f>'[1]Qc, 2020, Summer'!T10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.14301576321428572</v>
+        <v>-0.15890640357142857</v>
       </c>
       <c r="U10" s="1">
         <f>'[1]Qc, 2020, Summer'!U10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.15676148571428572</v>
+        <v>-0.17417942857142857</v>
       </c>
       <c r="V10" s="1">
         <f>'[1]Qc, 2020, Summer'!V10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.14218872107142858</v>
+        <v>-0.15798746785714285</v>
       </c>
       <c r="W10" s="1">
         <f>'[1]Qc, 2020, Summer'!W10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.10946458607142857</v>
+        <v>-0.12162731785714286</v>
       </c>
       <c r="X10" s="1">
         <f>'[1]Qc, 2020, Summer'!X10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.11923968214285714</v>
+        <v>-0.1324885357142857</v>
       </c>
       <c r="Y10" s="1">
         <f>'[1]Qc, 2020, Summer'!Y10*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.13034748214285716</v>
+        <v>-0.14483053571428572</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
@@ -20958,99 +20961,99 @@
       </c>
       <c r="B11" s="1">
         <f>'[1]Qc, 2020, Summer'!B11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.15501303642857142</v>
+        <v>-0.17223670714285713</v>
       </c>
       <c r="C11" s="1">
         <f>'[1]Qc, 2020, Summer'!C11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.14987603892857143</v>
+        <v>-0.16652893214285713</v>
       </c>
       <c r="D11" s="1">
         <f>'[1]Qc, 2020, Summer'!D11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.14686813928571427</v>
+        <v>-0.16318682142857141</v>
       </c>
       <c r="E11" s="1">
         <f>'[1]Qc, 2020, Summer'!E11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.14944318071428569</v>
+        <v>-0.16604797857142856</v>
       </c>
       <c r="F11" s="1">
         <f>'[1]Qc, 2020, Summer'!F11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.14088848464285714</v>
+        <v>-0.15654276071428572</v>
       </c>
       <c r="G11" s="1">
         <f>'[1]Qc, 2020, Summer'!G11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.13903134428571429</v>
+        <v>-0.15447927142857143</v>
       </c>
       <c r="H11" s="1">
         <f>'[1]Qc, 2020, Summer'!H11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.17750352857142856</v>
+        <v>-0.19722614285714285</v>
       </c>
       <c r="I11" s="1">
         <f>'[1]Qc, 2020, Summer'!I11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.15365615785714284</v>
+        <v>-0.17072906428571427</v>
       </c>
       <c r="J11" s="1">
         <f>'[1]Qc, 2020, Summer'!J11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.12690604928571428</v>
+        <v>-0.14100672142857143</v>
       </c>
       <c r="K11" s="1">
         <f>'[1]Qc, 2020, Summer'!K11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-8.9655287142857143E-2</v>
+        <v>-9.9616985714285705E-2</v>
       </c>
       <c r="L11" s="1">
         <f>'[1]Qc, 2020, Summer'!L11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.10276145035714288</v>
+        <v>-0.11417938928571431</v>
       </c>
       <c r="M11" s="1">
         <f>'[1]Qc, 2020, Summer'!M11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.10144734428571427</v>
+        <v>-0.11271927142857141</v>
       </c>
       <c r="N11" s="1">
         <f>'[1]Qc, 2020, Summer'!N11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.10097902285714284</v>
+        <v>-0.11219891428571427</v>
       </c>
       <c r="O11" s="1">
         <f>'[1]Qc, 2020, Summer'!O11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-9.678707035714286E-2</v>
+        <v>-0.10754118928571428</v>
       </c>
       <c r="P11" s="1">
         <f>'[1]Qc, 2020, Summer'!P11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.13302481821428572</v>
+        <v>-0.14780535357142857</v>
       </c>
       <c r="Q11" s="1">
         <f>'[1]Qc, 2020, Summer'!Q11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.12884849357142858</v>
+        <v>-0.14316499285714285</v>
       </c>
       <c r="R11" s="1">
         <f>'[1]Qc, 2020, Summer'!R11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.13198059000000001</v>
+        <v>-0.1466451</v>
       </c>
       <c r="S11" s="1">
         <f>'[1]Qc, 2020, Summer'!S11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.13797887785714288</v>
+        <v>-0.1533098642857143</v>
       </c>
       <c r="T11" s="1">
         <f>'[1]Qc, 2020, Summer'!T11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.14301576321428572</v>
+        <v>-0.15890640357142857</v>
       </c>
       <c r="U11" s="1">
         <f>'[1]Qc, 2020, Summer'!U11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.15676148571428572</v>
+        <v>-0.17417942857142857</v>
       </c>
       <c r="V11" s="1">
         <f>'[1]Qc, 2020, Summer'!V11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.14218872107142858</v>
+        <v>-0.15798746785714285</v>
       </c>
       <c r="W11" s="1">
         <f>'[1]Qc, 2020, Summer'!W11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.10946458607142857</v>
+        <v>-0.12162731785714286</v>
       </c>
       <c r="X11" s="1">
         <f>'[1]Qc, 2020, Summer'!X11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.11923968214285714</v>
+        <v>-0.1324885357142857</v>
       </c>
       <c r="Y11" s="1">
         <f>'[1]Qc, 2020, Summer'!Y11*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>-0.13034748214285716</v>
+        <v>-0.14483053571428572</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -21059,99 +21062,99 @@
       </c>
       <c r="B12" s="1">
         <f>'[1]Qc, 2020, Summer'!B12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.0358631064285715</v>
+        <v>1.1509590071428573</v>
       </c>
       <c r="C12" s="1">
         <f>'[1]Qc, 2020, Summer'!C12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.92564688857142863</v>
+        <v>1.0284965428571429</v>
       </c>
       <c r="D12" s="1">
         <f>'[1]Qc, 2020, Summer'!D12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.90527155392857139</v>
+        <v>1.0058572821428571</v>
       </c>
       <c r="E12" s="1">
         <f>'[1]Qc, 2020, Summer'!E12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.83588273999999996</v>
+        <v>0.92875859999999999</v>
       </c>
       <c r="F12" s="1">
         <f>'[1]Qc, 2020, Summer'!F12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.90715608321428565</v>
+        <v>1.0079512035714284</v>
       </c>
       <c r="G12" s="1">
         <f>'[1]Qc, 2020, Summer'!G12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.79955358749999994</v>
+        <v>0.88839287499999986</v>
       </c>
       <c r="H12" s="1">
         <f>'[1]Qc, 2020, Summer'!H12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.8497696950000001</v>
+        <v>0.94418855000000013</v>
       </c>
       <c r="I12" s="1">
         <f>'[1]Qc, 2020, Summer'!I12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.0975695653571429</v>
+        <v>1.2195217392857143</v>
       </c>
       <c r="J12" s="1">
         <f>'[1]Qc, 2020, Summer'!J12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.2848262267857142</v>
+        <v>1.4275846964285712</v>
       </c>
       <c r="K12" s="1">
         <f>'[1]Qc, 2020, Summer'!K12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.3279151667857145</v>
+        <v>1.4754612964285716</v>
       </c>
       <c r="L12" s="1">
         <f>'[1]Qc, 2020, Summer'!L12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.3828491482142857</v>
+        <v>1.5364990535714285</v>
       </c>
       <c r="M12" s="1">
         <f>'[1]Qc, 2020, Summer'!M12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.4040018096428573</v>
+        <v>1.5600020107142858</v>
       </c>
       <c r="N12" s="1">
         <f>'[1]Qc, 2020, Summer'!N12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.4046853917857143</v>
+        <v>1.5607615464285713</v>
       </c>
       <c r="O12" s="1">
         <f>'[1]Qc, 2020, Summer'!O12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.3840037614285714</v>
+        <v>1.537781957142857</v>
       </c>
       <c r="P12" s="1">
         <f>'[1]Qc, 2020, Summer'!P12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.2733474082142859</v>
+        <v>1.4148304535714287</v>
       </c>
       <c r="Q12" s="1">
         <f>'[1]Qc, 2020, Summer'!Q12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.2157520432142859</v>
+        <v>1.3508356035714286</v>
       </c>
       <c r="R12" s="1">
         <f>'[1]Qc, 2020, Summer'!R12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.1592291246428572</v>
+        <v>1.2880323607142858</v>
       </c>
       <c r="S12" s="1">
         <f>'[1]Qc, 2020, Summer'!S12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.1697067189285715</v>
+        <v>1.2996741321428571</v>
       </c>
       <c r="T12" s="1">
         <f>'[1]Qc, 2020, Summer'!T12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.1839314825000002</v>
+        <v>1.3154794250000001</v>
       </c>
       <c r="U12" s="1">
         <f>'[1]Qc, 2020, Summer'!U12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.1767238967857143</v>
+        <v>1.3074709964285713</v>
       </c>
       <c r="V12" s="1">
         <f>'[1]Qc, 2020, Summer'!V12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.1983940003571429</v>
+        <v>1.3315488892857144</v>
       </c>
       <c r="W12" s="1">
         <f>'[1]Qc, 2020, Summer'!W12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.2927654739285712</v>
+        <v>1.4364060821428568</v>
       </c>
       <c r="X12" s="1">
         <f>'[1]Qc, 2020, Summer'!X12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.1809953</v>
+        <v>1.312217</v>
       </c>
       <c r="Y12" s="1">
         <f>'[1]Qc, 2020, Summer'!Y12*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.11248163</v>
+        <v>1.2360906999999999</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -21160,99 +21163,99 @@
       </c>
       <c r="B13" s="1">
         <f>'[1]Qc, 2020, Summer'!B13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.56063230714285717</v>
+        <v>0.62292478571428578</v>
       </c>
       <c r="C13" s="1">
         <f>'[1]Qc, 2020, Summer'!C13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.56063230714285717</v>
+        <v>0.62292478571428578</v>
       </c>
       <c r="D13" s="1">
         <f>'[1]Qc, 2020, Summer'!D13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.5517540932142857</v>
+        <v>0.61306010357142859</v>
       </c>
       <c r="E13" s="1">
         <f>'[1]Qc, 2020, Summer'!E13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.53373857464285723</v>
+        <v>0.5930428607142858</v>
       </c>
       <c r="F13" s="1">
         <f>'[1]Qc, 2020, Summer'!F13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.52740964285714287</v>
+        <v>0.58601071428571427</v>
       </c>
       <c r="G13" s="1">
         <f>'[1]Qc, 2020, Summer'!G13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.42132142607142864</v>
+        <v>0.4681349178571429</v>
       </c>
       <c r="H13" s="1">
         <f>'[1]Qc, 2020, Summer'!H13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.38537074285714279</v>
+        <v>0.42818971428571423</v>
       </c>
       <c r="I13" s="1">
         <f>'[1]Qc, 2020, Summer'!I13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.59149214035714293</v>
+        <v>0.65721348928571433</v>
       </c>
       <c r="J13" s="1">
         <f>'[1]Qc, 2020, Summer'!J13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.69753984428571436</v>
+        <v>0.77504427142857146</v>
       </c>
       <c r="K13" s="1">
         <f>'[1]Qc, 2020, Summer'!K13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.7851539860714285</v>
+        <v>0.8723933178571428</v>
       </c>
       <c r="L13" s="1">
         <f>'[1]Qc, 2020, Summer'!L13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.8004903396428571</v>
+        <v>0.88943371071428567</v>
       </c>
       <c r="M13" s="1">
         <f>'[1]Qc, 2020, Summer'!M13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.89450718749999991</v>
+        <v>0.9938968749999999</v>
       </c>
       <c r="N13" s="1">
         <f>'[1]Qc, 2020, Summer'!N13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.88922399464285706</v>
+        <v>0.98802666071428558</v>
       </c>
       <c r="O13" s="1">
         <f>'[1]Qc, 2020, Summer'!O13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.89689895678571419</v>
+        <v>0.99655439642857124</v>
       </c>
       <c r="P13" s="1">
         <f>'[1]Qc, 2020, Summer'!P13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.84519973607142862</v>
+        <v>0.9391108178571429</v>
       </c>
       <c r="Q13" s="1">
         <f>'[1]Qc, 2020, Summer'!Q13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.83628523285714274</v>
+        <v>0.92920581428571414</v>
       </c>
       <c r="R13" s="1">
         <f>'[1]Qc, 2020, Summer'!R13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.67542707571428562</v>
+        <v>0.75047452857142849</v>
       </c>
       <c r="S13" s="1">
         <f>'[1]Qc, 2020, Summer'!S13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.61001123464285711</v>
+        <v>0.67779026071428572</v>
       </c>
       <c r="T13" s="1">
         <f>'[1]Qc, 2020, Summer'!T13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.60491868107142854</v>
+        <v>0.67213186785714285</v>
       </c>
       <c r="U13" s="1">
         <f>'[1]Qc, 2020, Summer'!U13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.58577282035714284</v>
+        <v>0.65085868928571422</v>
       </c>
       <c r="V13" s="1">
         <f>'[1]Qc, 2020, Summer'!V13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.59865532714285719</v>
+        <v>0.66517258571428572</v>
       </c>
       <c r="W13" s="1">
         <f>'[1]Qc, 2020, Summer'!W13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.62813980285714299</v>
+        <v>0.69793311428571436</v>
       </c>
       <c r="X13" s="1">
         <f>'[1]Qc, 2020, Summer'!X13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.61026900107142867</v>
+        <v>0.67807666785714293</v>
       </c>
       <c r="Y13" s="1">
         <f>'[1]Qc, 2020, Summer'!Y13*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.60393899571428578</v>
+        <v>0.67104332857142868</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -21261,99 +21264,99 @@
       </c>
       <c r="B14" s="1">
         <f>'[1]Qc, 2020, Summer'!B14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.89378251071428572</v>
+        <v>0.99309167857142855</v>
       </c>
       <c r="C14" s="1">
         <f>'[1]Qc, 2020, Summer'!C14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.0267218739285715</v>
+        <v>1.1408020821428573</v>
       </c>
       <c r="D14" s="1">
         <f>'[1]Qc, 2020, Summer'!D14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.67337551928571437</v>
+        <v>0.74819502142857153</v>
       </c>
       <c r="E14" s="1">
         <f>'[1]Qc, 2020, Summer'!E14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.91516129392857148</v>
+        <v>1.0168458821428572</v>
       </c>
       <c r="F14" s="1">
         <f>'[1]Qc, 2020, Summer'!F14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.83851706250000002</v>
+        <v>0.93168562499999996</v>
       </c>
       <c r="G14" s="1">
         <f>'[1]Qc, 2020, Summer'!G14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.81856420392857143</v>
+        <v>0.90951578214285711</v>
       </c>
       <c r="H14" s="1">
         <f>'[1]Qc, 2020, Summer'!H14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.99911928214285717</v>
+        <v>1.1101325357142857</v>
       </c>
       <c r="I14" s="1">
         <f>'[1]Qc, 2020, Summer'!I14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.97332002678571439</v>
+        <v>1.0814666964285715</v>
       </c>
       <c r="J14" s="1">
         <f>'[1]Qc, 2020, Summer'!J14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.0672796217857146</v>
+        <v>1.1858662464285716</v>
       </c>
       <c r="K14" s="1">
         <f>'[1]Qc, 2020, Summer'!K14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.0870113214285715</v>
+        <v>1.2077903571428572</v>
       </c>
       <c r="L14" s="1">
         <f>'[1]Qc, 2020, Summer'!L14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.98289073928571435</v>
+        <v>1.0921008214285715</v>
       </c>
       <c r="M14" s="1">
         <f>'[1]Qc, 2020, Summer'!M14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.0100297603571429</v>
+        <v>1.1222552892857143</v>
       </c>
       <c r="N14" s="1">
         <f>'[1]Qc, 2020, Summer'!N14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.0586641692857144</v>
+        <v>1.1762935214285715</v>
       </c>
       <c r="O14" s="1">
         <f>'[1]Qc, 2020, Summer'!O14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.0385111635714286</v>
+        <v>1.1539012928571428</v>
       </c>
       <c r="P14" s="1">
         <f>'[1]Qc, 2020, Summer'!P14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.0641840139285716</v>
+        <v>1.1824266821428573</v>
       </c>
       <c r="Q14" s="1">
         <f>'[1]Qc, 2020, Summer'!Q14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.1082767014285713</v>
+        <v>1.2314185571428569</v>
       </c>
       <c r="R14" s="1">
         <f>'[1]Qc, 2020, Summer'!R14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.1086436860714284</v>
+        <v>1.2318263178571427</v>
       </c>
       <c r="S14" s="1">
         <f>'[1]Qc, 2020, Summer'!S14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.0985616642857143</v>
+        <v>1.2206240714285714</v>
       </c>
       <c r="T14" s="1">
         <f>'[1]Qc, 2020, Summer'!T14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.0237587460714286</v>
+        <v>1.1375097178571429</v>
       </c>
       <c r="U14" s="1">
         <f>'[1]Qc, 2020, Summer'!U14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.1013323464285716</v>
+        <v>1.2237026071428574</v>
       </c>
       <c r="V14" s="1">
         <f>'[1]Qc, 2020, Summer'!V14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.111411173214286</v>
+        <v>1.2349013035714287</v>
       </c>
       <c r="W14" s="1">
         <f>'[1]Qc, 2020, Summer'!W14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.0344051192857147</v>
+        <v>1.1493390214285717</v>
       </c>
       <c r="X14" s="1">
         <f>'[1]Qc, 2020, Summer'!X14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>0.92228381999999998</v>
+        <v>1.0247598</v>
       </c>
       <c r="Y14" s="1">
         <f>'[1]Qc, 2020, Summer'!Y14*Main!$C$2*(1+[1]Main!$B$2)^(Main!$B$5-2020)</f>
-        <v>1.0237147007142855</v>
+        <v>1.1374607785714284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>